<commit_message>
feat: Update COVAX_AGG export config and package for v2.30 and add package for v2.33
</commit_message>
<xml_diff>
--- a/metadata/COVAX_AGG/COVAX_AGG_DASHBOARD_V1_DHIS2.30/reference.xlsx
+++ b/metadata/COVAX_AGG/COVAX_AGG_DASHBOARD_V1_DHIS2.30/reference.xlsx
@@ -491,7 +491,7 @@
         <v>Identifier</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>COVAX_AGG_DASHBOARD_V1.0_DHIS2.30_2021-01-26T15:05</v>
+        <v>COVAX_AGG_DASHBOARD_V1.0_DHIS2.30_2021-01-28T18:52</v>
       </c>
     </row>
   </sheetData>
@@ -861,7 +861,7 @@
         <v>Chart</v>
       </c>
       <c r="C18" s="4" t="str">
-        <v>COVAX - Number of people given 1st and last dose - this and last 6 months</v>
+        <v>COVAX - Number of people given 1st - this and last 6 months</v>
       </c>
       <c r="D18" s="4" t="str">
         <v>eLK1hVjcRMJ</v>
@@ -904,7 +904,7 @@
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
-    <col min="1" max="1" width="75.7109375" customWidth="1"/>
+    <col min="1" max="1" width="71.7109375" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="14.7109375" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" customWidth="1"/>
@@ -1010,13 +1010,13 @@
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>COVAX - Number of people given 1st and last dose - this and last 6 months</v>
+        <v>COVAX - Number of people given 1st - this and last 6 months</v>
       </c>
       <c r="B8" s="4" t="str">
         <v xml:space="preserve"> </v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>2021-01-21</v>
+        <v>2021-01-28</v>
       </c>
       <c r="D8" s="4" t="str">
         <v>NBIo8UnkJsU</v>
@@ -1131,7 +1131,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2021-01-19</v>
+        <v>2021-01-27</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>q24wzRQtygl</v>
@@ -1507,7 +1507,7 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
@@ -1541,12 +1541,23 @@
     </row>
     <row r="3">
       <c r="A3" s="5" t="str">
+        <v>COVAX capture</v>
+      </c>
+      <c r="B3" s="5" t="str">
+        <v>2021-01-20</v>
+      </c>
+      <c r="C3" s="5" t="str">
+        <v>I9x6Bd4MwXc</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="4" t="str">
         <v>COVAX access</v>
       </c>
-      <c r="B3" s="5" t="str">
+      <c r="B4" s="4" t="str">
         <v>2021-01-21</v>
       </c>
-      <c r="C3" s="5" t="str">
+      <c r="C4" s="4" t="str">
         <v>OeiDCnG3Pv2</v>
       </c>
     </row>
@@ -1860,13 +1871,13 @@
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>[CONFIG] &lt;60 years</v>
+        <v>[CONFIG] 0-59 years</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>&lt;60 y</v>
+        <v>0-59 y</v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>2021-01-18</v>
+        <v>2021-01-27</v>
       </c>
       <c r="D8" s="4" t="str">
         <v>fqborXHhXZG</v>
@@ -1908,7 +1919,7 @@
         <v>Contamination</v>
       </c>
       <c r="C11" s="5" t="str">
-        <v>2021-01-18</v>
+        <v>2021-01-28</v>
       </c>
       <c r="D11" s="5" t="str">
         <v>KS058ZLL570</v>
@@ -2038,7 +2049,7 @@
         <v>Age(&lt;60-60+years)</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>[CONFIG] &lt;60 years</v>
+        <v>[CONFIG] 0-59 years</v>
       </c>
     </row>
     <row r="8">
@@ -2144,7 +2155,7 @@
         <v/>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2021-01-21</v>
+        <v>2021-01-28</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2156,13 +2167,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J114"/>
+  <dimension ref="A1:J108"/>
   <sheetViews>
     <sheetView showGridLines="1" tabSelected="0" workbookViewId="0"/>
   </sheetViews>
   <cols>
     <col min="1" max="1" width="13.7109375" customWidth="1"/>
-    <col min="2" max="2" width="97.7109375" customWidth="1"/>
+    <col min="2" max="2" width="96.7109375" customWidth="1"/>
     <col min="3" max="3" width="52.7109375" customWidth="1"/>
     <col min="4" max="4" width="47.7109375" customWidth="1"/>
     <col min="5" max="5" width="90.7109375" customWidth="1"/>
@@ -2231,7 +2242,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I2" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J2" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2242,10 +2253,10 @@
         <v>AfDDi4x9jOt</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>[CONFIG] COVAX - Opening balance cold boxes</v>
+        <v>[CONFIG] COVAX - Opening balance cold box</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>Opening balance cold boxes</v>
+        <v>Opening balance cold box</v>
       </c>
       <c r="D3" s="5" t="str">
         <v>CVX_OPENING_BALANCE_COLD_BOXES</v>
@@ -2254,7 +2265,7 @@
         <v>Opening balance equals the physical 'stock on hand count' of the previous period</v>
       </c>
       <c r="F3" s="5" t="str">
-        <v>Opening balance cold boxes</v>
+        <v>Opening balance cold box</v>
       </c>
       <c r="G3" s="5" t="str">
         <v>1</v>
@@ -2263,7 +2274,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I3" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J3" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2274,16 +2285,16 @@
         <v>ANmlPnVtTTa</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>[CONFIG] COVAX - Stockout days - Vaccine3 vials</v>
+        <v>[CONFIG] COVAX - Stockout days - Vaccine 3 (vials)</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>Stockout days - Vaccine3 vials</v>
+        <v>Stockout days - Vaccine 3 (vials)</v>
       </c>
       <c r="D4" s="4" t="str">
         <v>CVX_STOCKOUT_DAYS_VACCINE3_VIALS</v>
       </c>
       <c r="E4" s="4" t="str">
-        <v xml:space="preserve"> Days the centre was stocked out of the item</v>
+        <v>Days the centre was stocked out of the item</v>
       </c>
       <c r="F4" s="4" t="str">
         <v>Stockout days - Vaccine3</v>
@@ -2295,7 +2306,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I4" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J4" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2327,7 +2338,7 @@
         <v>Percentage</v>
       </c>
       <c r="I5" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J5" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2335,31 +2346,31 @@
     </row>
     <row r="6">
       <c r="A6" s="4" t="str">
-        <v>AXQfVQKvZJu</v>
+        <v>b3znXSaQjkD</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>[CONFIG] COVAX - Target people with existing medical conditions given last dose</v>
+        <v>[CONFIG] COVAX - Proportion of staff available</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>People with existing conditions given last dose</v>
+        <v>Staff available (%)</v>
       </c>
       <c r="D6" s="4" t="str">
-        <v>CVX_PEOPLE_WITH_EXISTING_COND_LAST_DOSE</v>
+        <v>CVX_STAFF_AVAILABLE_%</v>
       </c>
       <c r="E6" s="4" t="str">
-        <v>People with underlying medical conditions given last dose</v>
+        <v>Proportion of staff available</v>
       </c>
       <c r="F6" s="4" t="str">
-        <v>Target people with underlying medical conditions given last dose</v>
+        <v>Staff available</v>
       </c>
       <c r="G6" s="4" t="str">
-        <v>1</v>
+        <v>Expected staff</v>
       </c>
       <c r="H6" s="4" t="str">
-        <v>Numerator only (number)</v>
+        <v>Percentage</v>
       </c>
       <c r="I6" s="4" t="str">
-        <v>2021-01-21</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J6" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2367,31 +2378,31 @@
     </row>
     <row r="7">
       <c r="A7" s="5" t="str">
-        <v>b3znXSaQjkD</v>
+        <v>B7vM2EWHmrP</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>[CONFIG] COVAX - Proportion of staff available</v>
+        <v>[CONFIG] COVAX - Stock at hand safety box</v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>Staff available (%)</v>
+        <v>Stock at hand safety box</v>
       </c>
       <c r="D7" s="5" t="str">
-        <v>CVX_STAFF_AVAILABLE_%</v>
+        <v>CVX_STOCK_AT_HAND_SAFETY_BOX</v>
       </c>
       <c r="E7" s="5" t="str">
-        <v>Proportion of staff available</v>
+        <v>Stock on-hand at the center after a physical stock count</v>
       </c>
       <c r="F7" s="5" t="str">
-        <v>Staff available</v>
+        <v>Stock on hand safety boxes</v>
       </c>
       <c r="G7" s="5" t="str">
-        <v xml:space="preserve">Expected staff </v>
+        <v>1</v>
       </c>
       <c r="H7" s="5" t="str">
-        <v>Percentage</v>
+        <v>Numerator only (number)</v>
       </c>
       <c r="I7" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J7" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2399,22 +2410,22 @@
     </row>
     <row r="8">
       <c r="A8" s="4" t="str">
-        <v>B7vM2EWHmrP</v>
+        <v>BbcV04tNF2n</v>
       </c>
       <c r="B8" s="4" t="str">
-        <v>[CONFIG] COVAX - Stock on hand safety boxes</v>
+        <v>[CONFIG] COVAX - Opening balance - Vaccine 2 (doses)</v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>Stock on hand safety boxes</v>
+        <v>Opening balance - Vaccine 2 (doses)</v>
       </c>
       <c r="D8" s="4" t="str">
-        <v>CVX_STOCK_ON_HAND_SAFETY_BOXES</v>
+        <v>CVX_OPENING_BALANCE_VACCINE2_DOSES</v>
       </c>
       <c r="E8" s="4" t="str">
-        <v xml:space="preserve">Stock on-hand at the center after a physical stock count </v>
+        <v>Opening balance equals the physical 'stock on hand count' of the previous day</v>
       </c>
       <c r="F8" s="4" t="str">
-        <v>Stock on hand safety boxes</v>
+        <v>Opening balance - Vaccine2 doses</v>
       </c>
       <c r="G8" s="4" t="str">
         <v>1</v>
@@ -2423,7 +2434,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I8" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J8" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2431,22 +2442,22 @@
     </row>
     <row r="9">
       <c r="A9" s="5" t="str">
-        <v>BbcV04tNF2n</v>
+        <v>BgtZgNWFVfb</v>
       </c>
       <c r="B9" s="5" t="str">
-        <v>[CONFIG] COVAX - Opening balance - Vaccine2 doses</v>
+        <v>[CONFIG] COVAX - Frontline healthcare workers given 2nd dose</v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>Opening balance - Vaccine2 doses</v>
+        <v>Frontline healthcare workers given 2nd dose</v>
       </c>
       <c r="D9" s="5" t="str">
-        <v>CVX_OPENING_BALANCE_VACCINE2_DOSES</v>
+        <v>CVX_FRONTLINE_HCW_2ND_DOSE</v>
       </c>
       <c r="E9" s="5" t="str">
-        <v>Opening balance equals the physical 'stock on hand count' of the previous day</v>
+        <v>Frontline healthcare workers given 2nd dose</v>
       </c>
       <c r="F9" s="5" t="str">
-        <v>Opening balance - Vaccine2 doses</v>
+        <v>Frontline healthcare workers given 2+ dose</v>
       </c>
       <c r="G9" s="5" t="str">
         <v>1</v>
@@ -2455,7 +2466,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I9" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J9" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2463,22 +2474,22 @@
     </row>
     <row r="10">
       <c r="A10" s="4" t="str">
-        <v>BgtZgNWFVfb</v>
+        <v>bmUnh1j8eUE</v>
       </c>
       <c r="B10" s="4" t="str">
-        <v>[CONFIG] COVAX - Frontline healthcare workers given 2+ dose</v>
+        <v>[CONFIG] COVAX - Distributed syringes with needle 1ml</v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>Frontline healthcare workers given 2+ dose</v>
+        <v>Distributed syringes with needle 1ml</v>
       </c>
       <c r="D10" s="4" t="str">
-        <v>CVX_FRONTLINE_HCW_2PLUS_DOSE</v>
+        <v>CVX_DISTRIBUTED_SYRINGES_WITH_ NEEDLE_1ML</v>
       </c>
       <c r="E10" s="4" t="str">
-        <v>Frontline healthcare workers given 2+ dose</v>
+        <v>Distributed to people receiving the items</v>
       </c>
       <c r="F10" s="4" t="str">
-        <v>Frontline healthcare workers given 2+ dose</v>
+        <v>Distributed syringes with needle 1ml</v>
       </c>
       <c r="G10" s="4" t="str">
         <v>1</v>
@@ -2487,7 +2498,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I10" s="4" t="str">
-        <v>2021-01-21</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J10" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2495,31 +2506,31 @@
     </row>
     <row r="11">
       <c r="A11" s="5" t="str">
-        <v>bmUnh1j8eUE</v>
+        <v>btAPoZyKLSW</v>
       </c>
       <c r="B11" s="5" t="str">
-        <v>[CONFIG] COVAX - Distributed syringes with needle 1ml</v>
+        <v>[CONFIG] COVAX - Drop out rates among frontline healthcare workers(%)</v>
       </c>
       <c r="C11" s="5" t="str">
-        <v>Distributed syringes with needle 1ml</v>
+        <v>Drop out rates among frontline HCW (%)</v>
       </c>
       <c r="D11" s="5" t="str">
-        <v>CVX_DISTRIBUTED_SYRINGES_WITH_ NEEDLE_1ML</v>
+        <v>CVX_DROPOUT_RATES_AMONG_FRONTLINE_HCW_%</v>
       </c>
       <c r="E11" s="5" t="str">
-        <v>Distributed to people receiving the items</v>
+        <v>(1st dose - 2nd dose)/1st dose</v>
       </c>
       <c r="F11" s="5" t="str">
-        <v>Distributed syringes with needle 1ml</v>
+        <v>Given 1st dose - Given second dose</v>
       </c>
       <c r="G11" s="5" t="str">
-        <v>1</v>
+        <v>Given 1st dose</v>
       </c>
       <c r="H11" s="5" t="str">
-        <v>Numerator only (number)</v>
+        <v>Percentage</v>
       </c>
       <c r="I11" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J11" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2527,31 +2538,31 @@
     </row>
     <row r="12">
       <c r="A12" s="4" t="str">
-        <v>btAPoZyKLSW</v>
+        <v>ByzkeCHudEH</v>
       </c>
       <c r="B12" s="4" t="str">
-        <v>[CONFIG] COVAX - Drop out rates among frontline healthcare workers(%)</v>
+        <v>[CONFIG] COVAX - Staff expected at PoC</v>
       </c>
       <c r="C12" s="4" t="str">
-        <v>Drop out rates among frontline HCW (%)</v>
+        <v>Staff expected at PoC</v>
       </c>
       <c r="D12" s="4" t="str">
-        <v>CVX_DROPOUT_RATES_AMONG_FRONTLINE_HCW_%</v>
+        <v>CVX_STAFF_EXPECTED_AT_POC</v>
       </c>
       <c r="E12" s="4" t="str">
-        <v>(1st dose - last dose)/1st dose</v>
+        <v>Staff expected at PoC during the reporting period</v>
       </c>
       <c r="F12" s="4" t="str">
-        <v>Given 1st dose - Given last dose</v>
+        <v>Staff expected at PoC</v>
       </c>
       <c r="G12" s="4" t="str">
-        <v>Given 1st dose</v>
+        <v>1</v>
       </c>
       <c r="H12" s="4" t="str">
-        <v>Percentage</v>
+        <v>Numerator only (number)</v>
       </c>
       <c r="I12" s="4" t="str">
-        <v>2021-01-21</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J12" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2559,31 +2570,31 @@
     </row>
     <row r="13">
       <c r="A13" s="5" t="str">
-        <v>ByzkeCHudEH</v>
+        <v>c4p6bfoOh0B</v>
       </c>
       <c r="B13" s="5" t="str">
-        <v>[CONFIG] COVAX - Staff expected at centre today</v>
+        <v>[CONFIG] COVAX - Drop out rates among essential workers(%)</v>
       </c>
       <c r="C13" s="5" t="str">
-        <v>Staff expected at centre today</v>
+        <v>Drop out rates among essential workers (%)</v>
       </c>
       <c r="D13" s="5" t="str">
-        <v>CVX_STAFF_EXPECTED_AT_CENTRE_TODAY</v>
+        <v>CVX_DROPOUT_RATES_AMONG_ESS_WORKERS_%</v>
       </c>
       <c r="E13" s="5" t="str">
-        <v>Staff expected at centre today</v>
+        <v>(1st dose - 2nd dose)/1st dose</v>
       </c>
       <c r="F13" s="5" t="str">
-        <v>Staff expected at centre today</v>
+        <v>Given 1st dose - Given second dose</v>
       </c>
       <c r="G13" s="5" t="str">
-        <v>1</v>
+        <v>Given 1st dose</v>
       </c>
       <c r="H13" s="5" t="str">
-        <v>Numerator only (number)</v>
+        <v>Percentage</v>
       </c>
       <c r="I13" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J13" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2591,31 +2602,31 @@
     </row>
     <row r="14">
       <c r="A14" s="4" t="str">
-        <v>c4p6bfoOh0B</v>
+        <v>cdLF5DVO45T</v>
       </c>
       <c r="B14" s="4" t="str">
-        <v>[CONFIG] COVAX - Drop out rates among essential workers(%)</v>
+        <v>[CONFIG] COVAX - Closed vials wastage (%)</v>
       </c>
       <c r="C14" s="4" t="str">
-        <v>Drop out rates among essential workers (%)</v>
+        <v>Closed vials wastage (%)</v>
       </c>
       <c r="D14" s="4" t="str">
-        <v>CVX_DROPOUT_RATES_AMONG_ESS_WORKERS_%</v>
+        <v>CVX_ CLOSED_VIALS_WASTAGE_%</v>
       </c>
       <c r="E14" s="4" t="str">
-        <v>(1st dose - last dose)/1st dose</v>
+        <v>(Discarded closed vial doses/Doses discarded)*100</v>
       </c>
       <c r="F14" s="4" t="str">
-        <v>Given 1st dose - Given last dose</v>
+        <v>Closed vial doses discarded</v>
       </c>
       <c r="G14" s="4" t="str">
-        <v>Given 1st dose</v>
+        <v>Discarded doses</v>
       </c>
       <c r="H14" s="4" t="str">
         <v>Percentage</v>
       </c>
       <c r="I14" s="4" t="str">
-        <v>2021-01-21</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J14" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2623,31 +2634,31 @@
     </row>
     <row r="15">
       <c r="A15" s="5" t="str">
-        <v>cdLF5DVO45T</v>
+        <v>cEUzKKCa7fv</v>
       </c>
       <c r="B15" s="5" t="str">
-        <v>[CONFIG] COVAX - Closed vials wastage (%)</v>
+        <v>[CONFIG] COVAX - Vaccine stock reporting rates</v>
       </c>
       <c r="C15" s="5" t="str">
-        <v>Closed vials wastage (%)</v>
+        <v>Vaccine stock reporting rates (%)</v>
       </c>
       <c r="D15" s="5" t="str">
-        <v>CVX_ CLOSED_VIALS_WASTAGE_%</v>
+        <v>CVX_VAC_STOCK_REPORTING_RATE_%</v>
       </c>
       <c r="E15" s="5" t="str">
-        <v>(Discarded closed vial doses/Doses discarded)*100</v>
+        <v>Proportion of all vaccination centres that submitted their report</v>
       </c>
       <c r="F15" s="5" t="str">
-        <v>Closed vial doses discarded</v>
+        <v>Actual reports received</v>
       </c>
       <c r="G15" s="5" t="str">
-        <v>Discarded doses</v>
+        <v>Expected reports</v>
       </c>
       <c r="H15" s="5" t="str">
         <v>Percentage</v>
       </c>
       <c r="I15" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J15" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2655,31 +2666,31 @@
     </row>
     <row r="16">
       <c r="A16" s="4" t="str">
-        <v>cEUzKKCa7fv</v>
+        <v>cSnIflt4J3h</v>
       </c>
       <c r="B16" s="4" t="str">
-        <v>[CONFIG] COVAX - Vaccine stock reporting rates</v>
+        <v>[CONFIG] COVAX - Redistributed - Vaccine1 doses</v>
       </c>
       <c r="C16" s="4" t="str">
-        <v>Vaccine stock reporting rates (%)</v>
+        <v>Redistributed - Vaccine1 doses</v>
       </c>
       <c r="D16" s="4" t="str">
-        <v>CVX_VAC_STOCK_REPORTING_RATE_%</v>
+        <v>CVX_REDISTRIBUTED_VACCINE1_DOSES</v>
       </c>
       <c r="E16" s="4" t="str">
-        <v xml:space="preserve">Proportion of all vaccination centres that submitted their report </v>
+        <v>Redistributed back into the supply chain and is no longer intended for the at the centre</v>
       </c>
       <c r="F16" s="4" t="str">
-        <v>Actual reports received</v>
+        <v>Redistributed - Vaccine1 doses</v>
       </c>
       <c r="G16" s="4" t="str">
-        <v>Expected reports</v>
+        <v>1</v>
       </c>
       <c r="H16" s="4" t="str">
-        <v>Percentage</v>
+        <v>Numerator only (number)</v>
       </c>
       <c r="I16" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J16" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2687,22 +2698,22 @@
     </row>
     <row r="17">
       <c r="A17" s="5" t="str">
-        <v>cSnIflt4J3h</v>
+        <v>CydbboFk0yH</v>
       </c>
       <c r="B17" s="5" t="str">
-        <v>[CONFIG] COVAX - Redistributed - Vaccine1 doses</v>
+        <v>[CONFIG] COVAX - Stock at hand - Vaccine 3 (doses)</v>
       </c>
       <c r="C17" s="5" t="str">
-        <v>Redistributed - Vaccine1 doses</v>
+        <v>Stock at hand - Vaccine 3 (doses)</v>
       </c>
       <c r="D17" s="5" t="str">
-        <v>CVX_REDISTRIBUTED_VACCINE1_DOSES</v>
+        <v>CVX_STOCK_AT_HAND_VACCINE3_DOSES</v>
       </c>
       <c r="E17" s="5" t="str">
-        <v>Redistributed back into the supply chain and is no longer intended for the at the centre</v>
+        <v>Stock on-hand at the center after a physical stock count</v>
       </c>
       <c r="F17" s="5" t="str">
-        <v>Redistributed - Vaccine1 doses</v>
+        <v>Stock on hand - Vaccine3 doses</v>
       </c>
       <c r="G17" s="5" t="str">
         <v>1</v>
@@ -2711,7 +2722,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I17" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J17" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2719,22 +2730,22 @@
     </row>
     <row r="18">
       <c r="A18" s="4" t="str">
-        <v>CydbboFk0yH</v>
+        <v>eA3THL80DDH</v>
       </c>
       <c r="B18" s="4" t="str">
-        <v>[CONFIG] COVAX - Stock on hand - Vaccine3 doses</v>
+        <v>[CONFIG] COVAX - Stockout days - Vaccine 1 (vials)</v>
       </c>
       <c r="C18" s="4" t="str">
-        <v>Stock on hand - Vaccine3 doses</v>
+        <v>Stockout days - Vaccine 1 (vials)</v>
       </c>
       <c r="D18" s="4" t="str">
-        <v>CVX_STOCK_ON_HAND_VACCINE3_DOSES</v>
+        <v>CVX_STOCKOUT_DAYS_VACCINE1_VIALS</v>
       </c>
       <c r="E18" s="4" t="str">
-        <v xml:space="preserve">Stock on-hand at the center after a physical stock count </v>
+        <v>Days the centre was stocked out of the item</v>
       </c>
       <c r="F18" s="4" t="str">
-        <v>Stock on hand - Vaccine3 doses</v>
+        <v>Stockout days - Vaccine1</v>
       </c>
       <c r="G18" s="4" t="str">
         <v>1</v>
@@ -2743,7 +2754,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I18" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J18" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2751,22 +2762,22 @@
     </row>
     <row r="19">
       <c r="A19" s="5" t="str">
-        <v>eA3THL80DDH</v>
+        <v>EMDTyzi8eMD</v>
       </c>
       <c r="B19" s="5" t="str">
-        <v>[CONFIG] COVAX - Stockout days - Vaccine1 vials</v>
+        <v>[CONFIG] COVAX - Stockout days syringes with needle 1ml</v>
       </c>
       <c r="C19" s="5" t="str">
-        <v>Stockout days - Vaccine1 vials</v>
+        <v>Stockout days syringes with needle 1ml</v>
       </c>
       <c r="D19" s="5" t="str">
-        <v>CVX_STOCKOUT_DAYS_VACCINE1_VIALS</v>
+        <v>CVX_STOCKOUT_DAYS_SYRINGES_WITH_ NEEDLE_1ML</v>
       </c>
       <c r="E19" s="5" t="str">
-        <v xml:space="preserve"> Days the centre was stocked out of the item</v>
+        <v>Days the facility was stocked out of the item</v>
       </c>
       <c r="F19" s="5" t="str">
-        <v>Stockout days - Vaccine1</v>
+        <v>Stockout days syringes with needle 1ml</v>
       </c>
       <c r="G19" s="5" t="str">
         <v>1</v>
@@ -2775,7 +2786,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I19" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J19" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2783,22 +2794,22 @@
     </row>
     <row r="20">
       <c r="A20" s="4" t="str">
-        <v>EMDTyzi8eMD</v>
+        <v>f1W0R9vbMEn</v>
       </c>
       <c r="B20" s="4" t="str">
-        <v>[CONFIG] COVAX - Stockout days syringes with needle 1ml</v>
+        <v>[CONFIG] COVAX - Stockout days vaccination cards</v>
       </c>
       <c r="C20" s="4" t="str">
-        <v>Stockout days syringes with needle 1ml</v>
+        <v>Stockout days vaccination cards</v>
       </c>
       <c r="D20" s="4" t="str">
-        <v>CVX_STOCKOUT_DAYS_SYRINGES_WITH_ NEEDLE_1ML</v>
+        <v>CVX_STOCKOUT_DAYS_CARDS</v>
       </c>
       <c r="E20" s="4" t="str">
         <v>Days the facility was stocked out of the item</v>
       </c>
       <c r="F20" s="4" t="str">
-        <v>Stockout days syringes with needle 1ml</v>
+        <v>Stockout days vaccination cards</v>
       </c>
       <c r="G20" s="4" t="str">
         <v>1</v>
@@ -2807,7 +2818,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I20" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J20" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2815,22 +2826,22 @@
     </row>
     <row r="21">
       <c r="A21" s="5" t="str">
-        <v>f1W0R9vbMEn</v>
+        <v>FE4mbnWq0rv</v>
       </c>
       <c r="B21" s="5" t="str">
-        <v>[CONFIG] COVAX - Stockout days vaccination cards</v>
+        <v>[CONFIG] COVAX - Discarded closed vials - Vaccine 2 (doses)</v>
       </c>
       <c r="C21" s="5" t="str">
-        <v>Stockout days vaccination cards</v>
+        <v>Discarded closed vials - Vaccine 2 (doses)</v>
       </c>
       <c r="D21" s="5" t="str">
-        <v>CVX_STOCKOUT_DAYS_CARDS</v>
+        <v>CVX_DISCARDED_VACCINE2_DOSES</v>
       </c>
       <c r="E21" s="5" t="str">
-        <v>Days the facility was stocked out of the item</v>
+        <v>Discarded due to expiry, damage, contamination and etc</v>
       </c>
       <c r="F21" s="5" t="str">
-        <v>Stockout days vaccination cards</v>
+        <v>Discarded - Vaccine2 doses</v>
       </c>
       <c r="G21" s="5" t="str">
         <v>1</v>
@@ -2839,7 +2850,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I21" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J21" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2847,31 +2858,31 @@
     </row>
     <row r="22">
       <c r="A22" s="4" t="str">
-        <v>FE4mbnWq0rv</v>
+        <v>ffjCEkN7xC2</v>
       </c>
       <c r="B22" s="4" t="str">
-        <v>[CONFIG] COVAX - Discarded - Vaccine2 doses</v>
+        <v>[CONFIG] COVAX - Stock discrepancy rate (%)</v>
       </c>
       <c r="C22" s="4" t="str">
-        <v>Discarded - Vaccine2 doses</v>
+        <v>Stock discrepancy rate (%)</v>
       </c>
       <c r="D22" s="4" t="str">
-        <v>CVX_DISCARDED_VACCINE2_DOSES</v>
+        <v>CVX_STOCK_DISCREPANCY_VIALS</v>
       </c>
       <c r="E22" s="4" t="str">
-        <v>Discarded due to expiry, damage, contamination and etc</v>
+        <v>(Closing balance-Stock on hand)/Stock on hand</v>
       </c>
       <c r="F22" s="4" t="str">
-        <v>Discarded - Vaccine2 doses</v>
+        <v>Closing balance-Stock at hand</v>
       </c>
       <c r="G22" s="4" t="str">
-        <v>1</v>
+        <v>Stock at hand</v>
       </c>
       <c r="H22" s="4" t="str">
-        <v>Numerator only (number)</v>
+        <v>Percentage</v>
       </c>
       <c r="I22" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J22" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2879,31 +2890,31 @@
     </row>
     <row r="23">
       <c r="A23" s="5" t="str">
-        <v>ffjCEkN7xC2</v>
+        <v>fQAVcB4dAQp</v>
       </c>
       <c r="B23" s="5" t="str">
-        <v>[CONFIG] COVAX - Stock discrepancy rate (%)</v>
+        <v>[CONFIG] COVAX - Redistributed vials</v>
       </c>
       <c r="C23" s="5" t="str">
-        <v>Stock discrepancy rate</v>
+        <v>Redistributed vials</v>
       </c>
       <c r="D23" s="5" t="str">
-        <v>CVX_STOCK_DISCREPANCY_VIALS</v>
+        <v>CVX_REDISTRIBUTED_VIALS</v>
       </c>
       <c r="E23" s="5" t="str">
-        <v>(Closing balance-Stock on hand)/Stock on hand</v>
+        <v>Redistributed back into the supply chain and is no longer intended for the at the centre</v>
       </c>
       <c r="F23" s="5" t="str">
-        <v>Closing balance-Stock on hand</v>
+        <v>Redistributed vials</v>
       </c>
       <c r="G23" s="5" t="str">
-        <v>Stock on hand</v>
+        <v>1</v>
       </c>
       <c r="H23" s="5" t="str">
-        <v>Percentage</v>
+        <v>Numerator only (number)</v>
       </c>
       <c r="I23" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J23" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2911,22 +2922,22 @@
     </row>
     <row r="24">
       <c r="A24" s="4" t="str">
-        <v>fQAVcB4dAQp</v>
+        <v>fySBzigjUbH</v>
       </c>
       <c r="B24" s="4" t="str">
-        <v>[CONFIG] COVAX - Redistributed vials</v>
+        <v>[CONFIG] COVAX - Closing balance vaccination cards</v>
       </c>
       <c r="C24" s="4" t="str">
-        <v>Redistributed vials</v>
+        <v>Closing balance vaccination cards</v>
       </c>
       <c r="D24" s="4" t="str">
-        <v>CVX_REDISTRIBUTED_VIALS</v>
+        <v>CVX_CLOSING_BALANCE_CARDS</v>
       </c>
       <c r="E24" s="4" t="str">
-        <v>Redistributed back into the supply chain and is no longer intended for the at the centre</v>
+        <v>(Opening balance+Received)-(Distributed+Redistributed+Discarded)</v>
       </c>
       <c r="F24" s="4" t="str">
-        <v>Redistributed vials</v>
+        <v>(Opening balance+Received)-(Distributed+Redistributed+Discarded)</v>
       </c>
       <c r="G24" s="4" t="str">
         <v>1</v>
@@ -2935,7 +2946,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I24" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J24" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2943,22 +2954,22 @@
     </row>
     <row r="25">
       <c r="A25" s="5" t="str">
-        <v>fySBzigjUbH</v>
+        <v>g2voTi7ZCxe</v>
       </c>
       <c r="B25" s="5" t="str">
-        <v>[CONFIG] COVAX - Closing balance vaccination cards</v>
+        <v>[CONFIG] COVAX - Opening balance - Vaccine 1 (doses)</v>
       </c>
       <c r="C25" s="5" t="str">
-        <v>Closing balance vaccination cards</v>
+        <v>Opening balance - Vaccine 1 (doses)</v>
       </c>
       <c r="D25" s="5" t="str">
-        <v>CVX_CLOSING_BALANCE_CARDS</v>
+        <v>CVX_OPENING_BALANCE_VACCINE1_DOSES</v>
       </c>
       <c r="E25" s="5" t="str">
-        <v>(Opening balance+Received)-(Distributed+Redistributed+Discarded)</v>
+        <v>Opening balance equals the physical 'stock on hand count of the previous day</v>
       </c>
       <c r="F25" s="5" t="str">
-        <v>(Opening balance+Received)-(Distributed+Redistributed+Discarded)</v>
+        <v>Opening balance - Vaccine1 doses</v>
       </c>
       <c r="G25" s="5" t="str">
         <v>1</v>
@@ -2967,7 +2978,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I25" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J25" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2975,22 +2986,22 @@
     </row>
     <row r="26">
       <c r="A26" s="4" t="str">
-        <v>g2voTi7ZCxe</v>
+        <v>G9jRzY6zmJg</v>
       </c>
       <c r="B26" s="4" t="str">
-        <v>[CONFIG] COVAX - Opening balance - Vaccine1 doses</v>
+        <v>[CONFIG] COVAX - Stock at hand vaccination cards</v>
       </c>
       <c r="C26" s="4" t="str">
-        <v>Opening balance - Vaccine1 doses</v>
+        <v>Stock at hand vaccination cards</v>
       </c>
       <c r="D26" s="4" t="str">
-        <v>CVX_OPENING_BALANCE_VACCINE1_DOSES</v>
+        <v>CVX_STOCK_AT_HAND_CARDS</v>
       </c>
       <c r="E26" s="4" t="str">
-        <v>Opening balance equals the physical 'stock on hand count of the previous day</v>
+        <v>Stock on-hand at the center after a physical stock count</v>
       </c>
       <c r="F26" s="4" t="str">
-        <v>Opening balance - Vaccine1 doses</v>
+        <v>Stock on hand vaccination cards</v>
       </c>
       <c r="G26" s="4" t="str">
         <v>1</v>
@@ -2999,7 +3010,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I26" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J26" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3007,22 +3018,22 @@
     </row>
     <row r="27">
       <c r="A27" s="5" t="str">
-        <v>G9jRzY6zmJg</v>
+        <v>gZEoyKpx4hE</v>
       </c>
       <c r="B27" s="5" t="str">
-        <v>[CONFIG] COVAX - Stock on hand vaccination cards</v>
+        <v>[CONFIG] COVAX - Essential workers given 2nd dose</v>
       </c>
       <c r="C27" s="5" t="str">
-        <v>Stock on hand vaccination cards</v>
+        <v>Essential workers given 2nd dose</v>
       </c>
       <c r="D27" s="5" t="str">
-        <v>CVX_STOCK_ON_HAND_CARDS</v>
+        <v>CVX_ESSENTIAL_WORKERS_2ND_DOSE</v>
       </c>
       <c r="E27" s="5" t="str">
-        <v xml:space="preserve">Stock on-hand at the center after a physical stock count </v>
+        <v>Essential workers given 2nd dose</v>
       </c>
       <c r="F27" s="5" t="str">
-        <v>Stock on hand vaccination cards</v>
+        <v>Essential workers given 2+ dose</v>
       </c>
       <c r="G27" s="5" t="str">
         <v>1</v>
@@ -3031,7 +3042,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I27" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J27" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3039,31 +3050,31 @@
     </row>
     <row r="28">
       <c r="A28" s="4" t="str">
-        <v>gZEoyKpx4hE</v>
+        <v>h3NchPC73cV</v>
       </c>
       <c r="B28" s="4" t="str">
-        <v>[CONFIG] COVAX - Essential workers given 2+ dose</v>
+        <v>[CONFIG] COVAX - Vaccination reporting rates</v>
       </c>
       <c r="C28" s="4" t="str">
-        <v>Essential workers given 2+ dose</v>
+        <v>Vaccination reporting rates (%)</v>
       </c>
       <c r="D28" s="4" t="str">
-        <v>CVX_ESSENTIAL_WORKERS_2PLUS_DOSE</v>
+        <v>CVX_VAC_REPORTING_RATE_%</v>
       </c>
       <c r="E28" s="4" t="str">
-        <v>Essential workers given 2+ dose</v>
+        <v>Proportion of all vaccination centres that submitted their report</v>
       </c>
       <c r="F28" s="4" t="str">
-        <v>Essential workers given 2+ dose</v>
+        <v>Actual reports received</v>
       </c>
       <c r="G28" s="4" t="str">
-        <v>1</v>
+        <v>Expected reports</v>
       </c>
       <c r="H28" s="4" t="str">
-        <v>Numerator only (number)</v>
+        <v>Percentage</v>
       </c>
       <c r="I28" s="4" t="str">
-        <v>2021-01-21</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J28" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3071,31 +3082,31 @@
     </row>
     <row r="29">
       <c r="A29" s="5" t="str">
-        <v>h3NchPC73cV</v>
+        <v>H6nsnH2w9A9</v>
       </c>
       <c r="B29" s="5" t="str">
-        <v>[CONFIG] COVAX - Vaccination reporting rates</v>
+        <v>[CONFIG] COVAX - Opening balance - Vaccine 3 (doses)</v>
       </c>
       <c r="C29" s="5" t="str">
-        <v>Vaccination reporting rates (%)</v>
+        <v>Opening balance - Vaccine 3 (doses)</v>
       </c>
       <c r="D29" s="5" t="str">
-        <v>CVX_VAC_REPORTING_RATE_%</v>
+        <v>CVX_OPENING_BALANCE_VACCINE3_DOSES</v>
       </c>
       <c r="E29" s="5" t="str">
-        <v xml:space="preserve">Proportion of all vaccination centres that submitted their report </v>
+        <v>Opening balance equals the physical 'stock on hand count' of the previous day</v>
       </c>
       <c r="F29" s="5" t="str">
-        <v>Actual reports received</v>
+        <v>Opening balance - Vaccine3 doses</v>
       </c>
       <c r="G29" s="5" t="str">
-        <v>Expected reports</v>
+        <v>1</v>
       </c>
       <c r="H29" s="5" t="str">
-        <v>Percentage</v>
+        <v>Numerator only (number)</v>
       </c>
       <c r="I29" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J29" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3103,22 +3114,22 @@
     </row>
     <row r="30">
       <c r="A30" s="4" t="str">
-        <v>H6nsnH2w9A9</v>
+        <v>hJKdezT5GcK</v>
       </c>
       <c r="B30" s="4" t="str">
-        <v>[CONFIG] COVAX - Opening balance - Vaccine3 doses</v>
+        <v>[CONFIG] COVAX - Closing balance - Vaccine 1 (doses)</v>
       </c>
       <c r="C30" s="4" t="str">
-        <v>Opening balance - Vaccine3 doses</v>
+        <v>Closing balance - Vaccine 1 (doses)</v>
       </c>
       <c r="D30" s="4" t="str">
-        <v>CVX_OPENING_BALANCE_VACCINE3_DOSES</v>
+        <v>CVX_CLOSING_BALANCE_VACCINE1_DOSES</v>
       </c>
       <c r="E30" s="4" t="str">
-        <v>Opening balance equals the physical 'stock on hand count' of the previous day</v>
+        <v>(Opening balance+Received)-(Distributed+Redistributed+Discarded)</v>
       </c>
       <c r="F30" s="4" t="str">
-        <v>Opening balance - Vaccine3 doses</v>
+        <v>(Opening balance+Received)-(Distributed+Redistributed+Discarded)</v>
       </c>
       <c r="G30" s="4" t="str">
         <v>1</v>
@@ -3127,7 +3138,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I30" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J30" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3135,22 +3146,22 @@
     </row>
     <row r="31">
       <c r="A31" s="5" t="str">
-        <v>hJKdezT5GcK</v>
+        <v>i0dG1vChnP6</v>
       </c>
       <c r="B31" s="5" t="str">
-        <v>[CONFIG] COVAX - Closing balance - Vaccine1 doses</v>
+        <v>[CONFIG] COVAX - Discarded closed vials - Vaccine 1 (doses)</v>
       </c>
       <c r="C31" s="5" t="str">
-        <v>Closing balance vials</v>
+        <v>Discarded closed vials - Vaccine 1 (doses)</v>
       </c>
       <c r="D31" s="5" t="str">
-        <v>CVX_CLOSING_BALANCE_VACCINE1_DOSES</v>
+        <v>CVX_DISCARDED_VACCINE1_DOSES</v>
       </c>
       <c r="E31" s="5" t="str">
-        <v>(Opening balance+Received)-(Distributed+Redistributed+Discarded)</v>
+        <v>Discarded due to expiry, damage, contamination and etc</v>
       </c>
       <c r="F31" s="5" t="str">
-        <v>(Opening balance+Received)-(Distributed+Redistributed+Discarded)</v>
+        <v>Discarded - Vaccine1 doses</v>
       </c>
       <c r="G31" s="5" t="str">
         <v>1</v>
@@ -3159,7 +3170,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I31" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J31" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3167,22 +3178,22 @@
     </row>
     <row r="32">
       <c r="A32" s="4" t="str">
-        <v>i0dG1vChnP6</v>
+        <v>iC5xj6Dqa0P</v>
       </c>
       <c r="B32" s="4" t="str">
-        <v>[CONFIG] COVAX - Discarded - Vaccine1 doses</v>
+        <v>[CONFIG] COVAX - Target frontline healthcare workers</v>
       </c>
       <c r="C32" s="4" t="str">
-        <v>Discarded - Vaccine1 doses</v>
+        <v>Target frontline healthcare workers</v>
       </c>
       <c r="D32" s="4" t="str">
-        <v>CVX_DISCARDED_VACCINE1_DOSES</v>
+        <v>CVX_TARGET_FRONTLINE_HCW</v>
       </c>
       <c r="E32" s="4" t="str">
-        <v>Discarded due to expiry, damage, contamination and etc</v>
+        <v>Target frontline healthcare workers</v>
       </c>
       <c r="F32" s="4" t="str">
-        <v>Discarded - Vaccine1 doses</v>
+        <v>Target frontline healthcare workers</v>
       </c>
       <c r="G32" s="4" t="str">
         <v>1</v>
@@ -3191,7 +3202,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I32" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J32" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3199,22 +3210,22 @@
     </row>
     <row r="33">
       <c r="A33" s="5" t="str">
-        <v>iC5xj6Dqa0P</v>
+        <v>ILLy5jdUwwE</v>
       </c>
       <c r="B33" s="5" t="str">
-        <v>[CONFIG] COVAX - Target frontline healthcare workers</v>
+        <v>[CONFIG] COVAX - Stockout days safety box</v>
       </c>
       <c r="C33" s="5" t="str">
-        <v>Target frontline healthcare workers</v>
+        <v>Stockout days safety box</v>
       </c>
       <c r="D33" s="5" t="str">
-        <v>CVX_TARGET_FRONTLINE_HCW</v>
+        <v>CVX_STOCKOUT_DAYS_SAFETY_BOX</v>
       </c>
       <c r="E33" s="5" t="str">
-        <v>Target frontline healthcare workers</v>
+        <v>Days the facility was stocked out of the item</v>
       </c>
       <c r="F33" s="5" t="str">
-        <v>Target frontline healthcare workers</v>
+        <v>Stockout days safety boxes</v>
       </c>
       <c r="G33" s="5" t="str">
         <v>1</v>
@@ -3223,7 +3234,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I33" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J33" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3231,31 +3242,31 @@
     </row>
     <row r="34">
       <c r="A34" s="4" t="str">
-        <v>ILLy5jdUwwE</v>
+        <v>Iv3tfc8gso7</v>
       </c>
       <c r="B34" s="4" t="str">
-        <v>[CONFIG] COVAX - Stockout days safety boxes</v>
+        <v>[CONFIG] COVAX - Vaccination reporting rates on time</v>
       </c>
       <c r="C34" s="4" t="str">
-        <v>Stockout days safety boxes</v>
+        <v>Vaccination reporting rates on time (%)</v>
       </c>
       <c r="D34" s="4" t="str">
-        <v>CVX_STOCKOUT_DAYS_SAFETY_BOXES</v>
+        <v>CVX_VAC_REPORTING_RATE_ONTIME_%</v>
       </c>
       <c r="E34" s="4" t="str">
-        <v>Days the facility was stocked out of the item</v>
+        <v>Proportion of all vaccination centres that submitted their report on time</v>
       </c>
       <c r="F34" s="4" t="str">
-        <v>Stockout days safety boxes</v>
+        <v>Actual reports received on time</v>
       </c>
       <c r="G34" s="4" t="str">
-        <v>1</v>
+        <v>Actual reports received</v>
       </c>
       <c r="H34" s="4" t="str">
-        <v>Numerator only (number)</v>
+        <v>Percentage</v>
       </c>
       <c r="I34" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J34" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3263,31 +3274,31 @@
     </row>
     <row r="35">
       <c r="A35" s="5" t="str">
-        <v>Iv3tfc8gso7</v>
+        <v>J4UW8FgK4vq</v>
       </c>
       <c r="B35" s="5" t="str">
-        <v>[CONFIG] COVAX - Vaccination reporting rates on time</v>
+        <v>[CONFIG] COVAX - Received vaccination cards</v>
       </c>
       <c r="C35" s="5" t="str">
-        <v>Vaccination reporting rates on time (%)</v>
+        <v>Received vaccination cards</v>
       </c>
       <c r="D35" s="5" t="str">
-        <v>CVX_VAC_REPORTING_RATE_ONTIME_%</v>
+        <v>CVX_RECEIVED_CARD</v>
       </c>
       <c r="E35" s="5" t="str">
-        <v>Proportion of all vaccination centres that submitted their report on time</v>
+        <v>Received at the centre</v>
       </c>
       <c r="F35" s="5" t="str">
-        <v>Actual reports received on time</v>
+        <v>Received vaccination cards</v>
       </c>
       <c r="G35" s="5" t="str">
-        <v>Actual reports received</v>
+        <v>1</v>
       </c>
       <c r="H35" s="5" t="str">
-        <v>Percentage</v>
+        <v>Numerator only (number)</v>
       </c>
       <c r="I35" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J35" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3295,31 +3306,31 @@
     </row>
     <row r="36">
       <c r="A36" s="4" t="str">
-        <v>J4UW8FgK4vq</v>
+        <v>j550fnnj9QU</v>
       </c>
       <c r="B36" s="4" t="str">
-        <v>[CONFIG] COVAX - Received vaccination cards</v>
+        <v>[CONFIG] COVAX - Vaccine 2 uptake (%)</v>
       </c>
       <c r="C36" s="4" t="str">
-        <v>Received vaccination cards</v>
+        <v>Vaccine 2 uptake (%)</v>
       </c>
       <c r="D36" s="4" t="str">
-        <v>CVX_RECEIVED_CARD</v>
+        <v>CVX_VACCINE2_UPTAKE_%</v>
       </c>
       <c r="E36" s="4" t="str">
-        <v>Received at the centre</v>
+        <v>Proportion of people given doses of vaccine2</v>
       </c>
       <c r="F36" s="4" t="str">
-        <v>Received vaccination cards</v>
+        <v>Vaccine2 doses given</v>
       </c>
       <c r="G36" s="4" t="str">
-        <v>1</v>
+        <v>Total doses of all vaccines given</v>
       </c>
       <c r="H36" s="4" t="str">
-        <v>Numerator only (number)</v>
+        <v>Percentage</v>
       </c>
       <c r="I36" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J36" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3327,31 +3338,31 @@
     </row>
     <row r="37">
       <c r="A37" s="5" t="str">
-        <v>j550fnnj9QU</v>
+        <v>jayuvPfIQBz</v>
       </c>
       <c r="B37" s="5" t="str">
-        <v>[CONFIG] COVAX - Vaccine2 uptake (%)</v>
+        <v>[CONFIG] COVAX - Received cold box</v>
       </c>
       <c r="C37" s="5" t="str">
-        <v>Vaccine2 uptake (%)</v>
+        <v>Received cold box</v>
       </c>
       <c r="D37" s="5" t="str">
-        <v>CVX_VACCINE2_UPTAKE_%</v>
+        <v>CVX_RECEIVED_COLD_BOX</v>
       </c>
       <c r="E37" s="5" t="str">
-        <v>Proportion of people given doses of vaccine2</v>
+        <v>Received at the centre</v>
       </c>
       <c r="F37" s="5" t="str">
-        <v>Vaccine2 doses given</v>
+        <v>Received cold boxes</v>
       </c>
       <c r="G37" s="5" t="str">
-        <v>Total doses of all vaccines given</v>
+        <v>1</v>
       </c>
       <c r="H37" s="5" t="str">
-        <v>Percentage</v>
+        <v>Numerator only (number)</v>
       </c>
       <c r="I37" s="5" t="str">
-        <v>2021-01-21</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J37" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3359,22 +3370,22 @@
     </row>
     <row r="38">
       <c r="A38" s="4" t="str">
-        <v>jayuvPfIQBz</v>
+        <v>jFlfqS1M9Hj</v>
       </c>
       <c r="B38" s="4" t="str">
-        <v>[CONFIG] COVAX - Received cold boxes</v>
+        <v>[CONFIG] COVAX - Staff available at PoC</v>
       </c>
       <c r="C38" s="4" t="str">
-        <v>Received cold boxes</v>
+        <v>Staff available at PoC</v>
       </c>
       <c r="D38" s="4" t="str">
-        <v>CVX_RECEIVED_COLD_BOXES</v>
+        <v>CVX_STAFF_AVAILABLE_AT_POC</v>
       </c>
       <c r="E38" s="4" t="str">
-        <v>Received at the centre</v>
+        <v>Staff available at PoC during the reporting period</v>
       </c>
       <c r="F38" s="4" t="str">
-        <v>Received cold boxes</v>
+        <v>Staff available at PoC</v>
       </c>
       <c r="G38" s="4" t="str">
         <v>1</v>
@@ -3383,7 +3394,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I38" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J38" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3391,31 +3402,31 @@
     </row>
     <row r="39">
       <c r="A39" s="5" t="str">
-        <v>jFlfqS1M9Hj</v>
+        <v>k9kIyVQEc0o</v>
       </c>
       <c r="B39" s="5" t="str">
-        <v>[CONFIG] COVAX - Staff available at centre today</v>
+        <v>[CONFIG] COVAX - Wastage rate (%)</v>
       </c>
       <c r="C39" s="5" t="str">
-        <v>Staff available at centre today</v>
+        <v>Wastage rate (%)</v>
       </c>
       <c r="D39" s="5" t="str">
-        <v>CVX_STAFF_AVAILABLE_AT_CENTRE_TODAY</v>
+        <v>CVX_ WASTAGE_RATE_%</v>
       </c>
       <c r="E39" s="5" t="str">
-        <v>Staff available at centre today</v>
+        <v>(Discarded/Used)*100</v>
       </c>
       <c r="F39" s="5" t="str">
-        <v>Staff available at centre today</v>
+        <v>Discarded doses</v>
       </c>
       <c r="G39" s="5" t="str">
-        <v>1</v>
+        <v>Used doses=(Opening balance+Received)-(Redistributed+Stock on hand)</v>
       </c>
       <c r="H39" s="5" t="str">
-        <v>Numerator only (number)</v>
+        <v>Percentage</v>
       </c>
       <c r="I39" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J39" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3423,31 +3434,31 @@
     </row>
     <row r="40">
       <c r="A40" s="4" t="str">
-        <v>k9kIyVQEc0o</v>
+        <v>Kkbt3LgbCbD</v>
       </c>
       <c r="B40" s="4" t="str">
-        <v>[CONFIG] COVAX - Wastage rate (%)</v>
+        <v>[CONFIG] COVAX - Doses per vial - Vaccine 3</v>
       </c>
       <c r="C40" s="4" t="str">
-        <v>Wastage rate (%)</v>
+        <v>Doses per vial - Vaccine 3</v>
       </c>
       <c r="D40" s="4" t="str">
-        <v>CVX_ WASTAGE_RATE_%</v>
+        <v>CVX_DOSES_IN_A_VIAL_VACCINE3</v>
       </c>
       <c r="E40" s="4" t="str">
-        <v>(Discarded/Used)*100</v>
+        <v>Number of doses in a vial - Vaccine3</v>
       </c>
       <c r="F40" s="4" t="str">
-        <v>Discarded doses</v>
+        <v>Doses in a vial - Vaccine3</v>
       </c>
       <c r="G40" s="4" t="str">
-        <v>Used doses=(Opening balance+Received)-(Redistributed+Stock on hand)</v>
+        <v>1</v>
       </c>
       <c r="H40" s="4" t="str">
-        <v>Percentage</v>
+        <v>Numerator only (number)</v>
       </c>
       <c r="I40" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J40" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3455,22 +3466,22 @@
     </row>
     <row r="41">
       <c r="A41" s="5" t="str">
-        <v>Kkbt3LgbCbD</v>
+        <v>KLFHy7LdaEp</v>
       </c>
       <c r="B41" s="5" t="str">
-        <v>[CONFIG] COVAX - Doses in a vial - Vaccine3</v>
+        <v>[CONFIG] COVAX - Received - Vaccine 2 (doses)</v>
       </c>
       <c r="C41" s="5" t="str">
-        <v>Doses in a vial - Vaccine3</v>
+        <v>Received - Vaccine 2 (doses)</v>
       </c>
       <c r="D41" s="5" t="str">
-        <v>CVX_DOSES_IN_A_VIAL_VACCINE3</v>
+        <v>CVX_RECEIVED_VACCINE2_DOSES</v>
       </c>
       <c r="E41" s="5" t="str">
-        <v>Number of doses in a vial - Vaccine3</v>
+        <v>Received at the centre</v>
       </c>
       <c r="F41" s="5" t="str">
-        <v>Doses in a vial - Vaccine3</v>
+        <v>Received - Vaccine2 doses</v>
       </c>
       <c r="G41" s="5" t="str">
         <v>1</v>
@@ -3479,7 +3490,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I41" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J41" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3487,22 +3498,22 @@
     </row>
     <row r="42">
       <c r="A42" s="4" t="str">
-        <v>KLFHy7LdaEp</v>
+        <v>kx79vq5XdQd</v>
       </c>
       <c r="B42" s="4" t="str">
-        <v>[CONFIG] COVAX - Received - Vaccine2 doses</v>
+        <v>[CONFIG] COVAX - Closing balance syringes with needle 1ml</v>
       </c>
       <c r="C42" s="4" t="str">
-        <v>Received - Vaccine2 doses</v>
+        <v>Closing balance syringes with needle 1ml</v>
       </c>
       <c r="D42" s="4" t="str">
-        <v>CVX_RECEIVED_VACCINE2_DOSES</v>
+        <v>CVX_CLOSING_BALANCE_SYRINGES_WITH_ NEEDLE_1ML</v>
       </c>
       <c r="E42" s="4" t="str">
-        <v>Received at the centre</v>
+        <v>(Opening balance+Received)-(Distributed+Redistributed+Discarded)</v>
       </c>
       <c r="F42" s="4" t="str">
-        <v>Received - Vaccine2 doses</v>
+        <v>(Opening balance+Received)-(Distributed+Redistributed+Discarded)</v>
       </c>
       <c r="G42" s="4" t="str">
         <v>1</v>
@@ -3511,7 +3522,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I42" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J42" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3519,22 +3530,22 @@
     </row>
     <row r="43">
       <c r="A43" s="5" t="str">
-        <v>ktUQ6Yk8Ztv</v>
+        <v>lGv5kC9pLPI</v>
       </c>
       <c r="B43" s="5" t="str">
-        <v>[CONFIG] COVAX - Target people given last dose</v>
+        <v>[CONFIG] COVAX - Discarded closed vials - Vaccine 1</v>
       </c>
       <c r="C43" s="5" t="str">
-        <v>Target people given last dose</v>
+        <v>Discarded closed vials - Vaccine 1</v>
       </c>
       <c r="D43" s="5" t="str">
-        <v>CVX_PEOPLE_LAST_DOSE</v>
+        <v>CVX_DISCARDED__OPEN_VIALS_VACCINE1</v>
       </c>
       <c r="E43" s="5" t="str">
-        <v>Target people vaccinated last dose</v>
+        <v>Discarded due to expiry, damage, contamination and etc</v>
       </c>
       <c r="F43" s="5" t="str">
-        <v>Target people given last dose</v>
+        <v>Discarded closed vials - Vaccine 1</v>
       </c>
       <c r="G43" s="5" t="str">
         <v>1</v>
@@ -3543,7 +3554,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I43" s="5" t="str">
-        <v>2021-01-21</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J43" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3551,31 +3562,31 @@
     </row>
     <row r="44">
       <c r="A44" s="4" t="str">
-        <v>kx79vq5XdQd</v>
+        <v>LgvcCkQIQ44</v>
       </c>
       <c r="B44" s="4" t="str">
-        <v>[CONFIG] COVAX - Closing balance syringes with needle 1ml</v>
+        <v>[CONFIG] COVAX - Opened vials wastage (%)</v>
       </c>
       <c r="C44" s="4" t="str">
-        <v>Closing balance syringes with needle 1ml</v>
+        <v>Opened vials wastage (%)</v>
       </c>
       <c r="D44" s="4" t="str">
-        <v>CVX_CLOSING_BALANCE_SYRINGES_WITH_ NEEDLE_1ML</v>
+        <v>CVX_ OPENED_VIALS_WASTAGE_%</v>
       </c>
       <c r="E44" s="4" t="str">
-        <v>(Opening balance+Received)-(Distributed+Redistributed+Discarded)</v>
+        <v>(Discarded open vial doses/Doses discarded)*100</v>
       </c>
       <c r="F44" s="4" t="str">
-        <v>(Opening balance+Received)-(Distributed+Redistributed+Discarded)</v>
+        <v>Opened vial doses discarded</v>
       </c>
       <c r="G44" s="4" t="str">
-        <v>1</v>
+        <v>Discarded doses</v>
       </c>
       <c r="H44" s="4" t="str">
-        <v>Numerator only (number)</v>
+        <v>Percentage</v>
       </c>
       <c r="I44" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J44" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3583,22 +3594,22 @@
     </row>
     <row r="45">
       <c r="A45" s="5" t="str">
-        <v>lGv5kC9pLPI</v>
+        <v>lXV4Lk0aah6</v>
       </c>
       <c r="B45" s="5" t="str">
-        <v>[CONFIG] COVAX - Discarded vials</v>
+        <v>[CONFIG] COVAX - Distributed vials</v>
       </c>
       <c r="C45" s="5" t="str">
-        <v>Discarded vials</v>
+        <v>Distributed vials</v>
       </c>
       <c r="D45" s="5" t="str">
-        <v>CVX_DISCARDED_VIALS</v>
+        <v>CVX_DISTRIBUTED_VIALS</v>
       </c>
       <c r="E45" s="5" t="str">
-        <v>Discarded due to expiry, damage, contamination and etc</v>
+        <v>Distributed to people receiving the items</v>
       </c>
       <c r="F45" s="5" t="str">
-        <v>Discarded vials</v>
+        <v>Distributed vials</v>
       </c>
       <c r="G45" s="5" t="str">
         <v>1</v>
@@ -3607,7 +3618,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I45" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J45" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3615,31 +3626,31 @@
     </row>
     <row r="46">
       <c r="A46" s="4" t="str">
-        <v>LgvcCkQIQ44</v>
+        <v>mQYStz4mXT5</v>
       </c>
       <c r="B46" s="4" t="str">
-        <v>[CONFIG] COVAX - Opened vials wastage (%)</v>
+        <v>[CONFIG] COVAX - Target people with existing medical conditions</v>
       </c>
       <c r="C46" s="4" t="str">
-        <v>Opened vials wastage (%)</v>
+        <v>Target people with existing medical conditions</v>
       </c>
       <c r="D46" s="4" t="str">
-        <v>CVX_ OPENED_VIALS_WASTAGE_%</v>
+        <v>CVX_TARGET_PEOPLE_WITH_EXISTING_CONDITIONS</v>
       </c>
       <c r="E46" s="4" t="str">
-        <v>(Discarded open vial doses/Doses discarded)*100</v>
+        <v>Target people with existing medical conditions</v>
       </c>
       <c r="F46" s="4" t="str">
-        <v>Opened vial doses discarded</v>
+        <v>Target people with existing medical conditions</v>
       </c>
       <c r="G46" s="4" t="str">
-        <v>Discarded doses</v>
+        <v>1</v>
       </c>
       <c r="H46" s="4" t="str">
-        <v>Percentage</v>
+        <v>Numerator only (number)</v>
       </c>
       <c r="I46" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J46" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3647,22 +3658,22 @@
     </row>
     <row r="47">
       <c r="A47" s="5" t="str">
-        <v>lXV4Lk0aah6</v>
+        <v>MRUsCIsRdps</v>
       </c>
       <c r="B47" s="5" t="str">
-        <v>[CONFIG] COVAX - Distributed vials</v>
+        <v>[CONFIG] COVAX - Distributed - Vaccine 2 (doses)</v>
       </c>
       <c r="C47" s="5" t="str">
-        <v>Distributed vials</v>
+        <v>Distributed - Vaccine 2 (doses)</v>
       </c>
       <c r="D47" s="5" t="str">
-        <v>CVX_DISTRIBUTED_VIALS</v>
+        <v>CVX_DISTRIBUTED_VACCINE2_DOSES</v>
       </c>
       <c r="E47" s="5" t="str">
-        <v>Distributed to people receiving the items</v>
+        <v>Distributed to people receiving the vaccines</v>
       </c>
       <c r="F47" s="5" t="str">
-        <v>Distributed vials</v>
+        <v>Distributed - Vaccine2 doses</v>
       </c>
       <c r="G47" s="5" t="str">
         <v>1</v>
@@ -3671,7 +3682,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I47" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J47" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3679,22 +3690,22 @@
     </row>
     <row r="48">
       <c r="A48" s="4" t="str">
-        <v>mQYStz4mXT5</v>
+        <v>N4iXbeP3T5O</v>
       </c>
       <c r="B48" s="4" t="str">
-        <v>[CONFIG] COVAX - Target people with existing medical conditions</v>
+        <v>[CONFIG] COVAX - Closing balance - Vaccine 2 (vials)</v>
       </c>
       <c r="C48" s="4" t="str">
-        <v>Target people with existing medical conditions</v>
+        <v>Closing balance - Vaccine 2 (vials)</v>
       </c>
       <c r="D48" s="4" t="str">
-        <v>CVX_TARGET_PEOPLE_WITH_EXISTING_CONDITIONS</v>
+        <v>CVX_CLOSING_BALANCE_VACCINE2_VIALS</v>
       </c>
       <c r="E48" s="4" t="str">
-        <v>Target people with existing medical conditions</v>
+        <v>(Opening balance+Received)-(Distributed+Redistributed+Discarded)</v>
       </c>
       <c r="F48" s="4" t="str">
-        <v>Target people with existing medical conditions</v>
+        <v>(Opening balance+Received)-(Distributed+Redistributed+Discarded)</v>
       </c>
       <c r="G48" s="4" t="str">
         <v>1</v>
@@ -3703,7 +3714,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I48" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J48" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3711,22 +3722,22 @@
     </row>
     <row r="49">
       <c r="A49" s="5" t="str">
-        <v>MRUsCIsRdps</v>
+        <v>N4O2KBFP7Ze</v>
       </c>
       <c r="B49" s="5" t="str">
-        <v>[CONFIG] COVAX - Distributed - Vaccine2 doses</v>
+        <v>[CONFIG] COVAX - Received syringes with needle 1ml</v>
       </c>
       <c r="C49" s="5" t="str">
-        <v>Distributed - Vaccine2 doses</v>
+        <v>Received syringes with needle 1ml</v>
       </c>
       <c r="D49" s="5" t="str">
-        <v>CVX_DISTRIBUTED_VACCINE2_DOSES</v>
+        <v>CVX_RECEIVED_SYRINGES_WITH_ NEEDLE_1ML</v>
       </c>
       <c r="E49" s="5" t="str">
-        <v>Distributed to people receiving the vaccines</v>
+        <v>Received at the centre</v>
       </c>
       <c r="F49" s="5" t="str">
-        <v>Distributed - Vaccine2 doses</v>
+        <v>Received syringes with needle 1ml</v>
       </c>
       <c r="G49" s="5" t="str">
         <v>1</v>
@@ -3735,7 +3746,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I49" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J49" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3743,22 +3754,22 @@
     </row>
     <row r="50">
       <c r="A50" s="4" t="str">
-        <v>N4iXbeP3T5O</v>
+        <v>n5u7G8DQYNJ</v>
       </c>
       <c r="B50" s="4" t="str">
-        <v>[CONFIG] COVAX - Closing balance - Vaccine2 vials</v>
+        <v>[CONFIG] COVAX - AEFIs by vaccine and severity</v>
       </c>
       <c r="C50" s="4" t="str">
-        <v>Closing balance - Vaccine2 vials</v>
+        <v>AEFIs by vaccine and severity</v>
       </c>
       <c r="D50" s="4" t="str">
-        <v>CVX_CLOSING_BALANCE_VACCINE2_VIALS</v>
+        <v>CVX_AEFIS_BY_VACCINE_AND_SEVERITY</v>
       </c>
       <c r="E50" s="4" t="str">
-        <v>(Opening balance+Received)-(Distributed+Redistributed+Discarded)</v>
+        <v>AEFIs by vaccine and severity</v>
       </c>
       <c r="F50" s="4" t="str">
-        <v>(Opening balance+Received)-(Distributed+Redistributed+Discarded)</v>
+        <v>AEFIs by vaccine and severity</v>
       </c>
       <c r="G50" s="4" t="str">
         <v>1</v>
@@ -3767,7 +3778,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I50" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J50" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3775,22 +3786,22 @@
     </row>
     <row r="51">
       <c r="A51" s="5" t="str">
-        <v>N4O2KBFP7Ze</v>
+        <v>nO5aJYGv9qb</v>
       </c>
       <c r="B51" s="5" t="str">
-        <v>[CONFIG] COVAX - Received syringes with needle 1ml</v>
+        <v>[CONFIG] COVAX - Received - Vaccine 3 (doses)</v>
       </c>
       <c r="C51" s="5" t="str">
-        <v>Received syringes with needle 1ml</v>
+        <v>Received - Vaccine 3 (doses)</v>
       </c>
       <c r="D51" s="5" t="str">
-        <v>CVX_RECEIVED_SYRINGES_WITH_ NEEDLE_1ML</v>
+        <v>CVX_RECEIVED_VACCINE3_DOSES</v>
       </c>
       <c r="E51" s="5" t="str">
         <v>Received at the centre</v>
       </c>
       <c r="F51" s="5" t="str">
-        <v>Received syringes with needle 1ml</v>
+        <v>Received - Vaccine3 doses</v>
       </c>
       <c r="G51" s="5" t="str">
         <v>1</v>
@@ -3799,7 +3810,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I51" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J51" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3807,22 +3818,22 @@
     </row>
     <row r="52">
       <c r="A52" s="4" t="str">
-        <v>n5u7G8DQYNJ</v>
+        <v>NtkYtrGGzGV</v>
       </c>
       <c r="B52" s="4" t="str">
-        <v>[CONFIG] COVAX - AEFIs by vaccine and severity</v>
+        <v>[CONFIG] COVAX - Essential workers given 1st dose</v>
       </c>
       <c r="C52" s="4" t="str">
-        <v>AEFIs by vaccine and severity</v>
+        <v>Essential workers given 1st dose</v>
       </c>
       <c r="D52" s="4" t="str">
-        <v>CVX_AEFIS_BY_VACCINE_AND_SEVERITY</v>
+        <v>CVX_ESSENTIAL_WORKERS_1ST_DOSE</v>
       </c>
       <c r="E52" s="4" t="str">
-        <v>AEFIs by vaccine and severity</v>
+        <v>Essential workers given 1st dose</v>
       </c>
       <c r="F52" s="4" t="str">
-        <v>AEFIs by vaccine and severity</v>
+        <v>Essential workers given 1st dose</v>
       </c>
       <c r="G52" s="4" t="str">
         <v>1</v>
@@ -3831,7 +3842,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I52" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J52" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3839,22 +3850,22 @@
     </row>
     <row r="53">
       <c r="A53" s="5" t="str">
-        <v>nO5aJYGv9qb</v>
+        <v>o2sAk0ai7X9</v>
       </c>
       <c r="B53" s="5" t="str">
-        <v>[CONFIG] COVAX - Received - Vaccine3 doses</v>
+        <v>[CONFIG] COVAX - Stock at hand - Vaccine 1 (doses)</v>
       </c>
       <c r="C53" s="5" t="str">
-        <v>Received - Vaccine3 doses</v>
+        <v>Stock at hand - Vaccine 1 (doses)</v>
       </c>
       <c r="D53" s="5" t="str">
-        <v>CVX_RECEIVED_VACCINE3_DOSES</v>
+        <v>CVX_STOCK_AT_HAND_VACCINE1_DOSES</v>
       </c>
       <c r="E53" s="5" t="str">
-        <v>Received at the centre</v>
+        <v>Stock on-hand at the center after a physical stock count</v>
       </c>
       <c r="F53" s="5" t="str">
-        <v>Received - Vaccine3 doses</v>
+        <v>Stock on hand - Vaccine1 doses</v>
       </c>
       <c r="G53" s="5" t="str">
         <v>1</v>
@@ -3863,7 +3874,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I53" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J53" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3871,22 +3882,22 @@
     </row>
     <row r="54">
       <c r="A54" s="4" t="str">
-        <v>NtkYtrGGzGV</v>
+        <v>O9HPe4hooiB</v>
       </c>
       <c r="B54" s="4" t="str">
-        <v>[CONFIG] COVAX - Essential workers given 1st dose</v>
+        <v>[CONFIG] COVAX - Doses discarded by reasons</v>
       </c>
       <c r="C54" s="4" t="str">
-        <v>Essential workers given 1st dose</v>
+        <v>Doses discarded by reasons</v>
       </c>
       <c r="D54" s="4" t="str">
-        <v>CVX_ESSENTIAL_WORKERS_1ST_DOSE</v>
+        <v>CVX_DOSES_DISCARDED_BY_REASONS</v>
       </c>
       <c r="E54" s="4" t="str">
-        <v>Essential workers given 1st dose</v>
+        <v>Discarded due to expiry, damage, contamination and etc</v>
       </c>
       <c r="F54" s="4" t="str">
-        <v>Essential workers given 1st dose</v>
+        <v>Vials discarded by reasons</v>
       </c>
       <c r="G54" s="4" t="str">
         <v>1</v>
@@ -3895,7 +3906,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I54" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J54" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3903,22 +3914,22 @@
     </row>
     <row r="55">
       <c r="A55" s="5" t="str">
-        <v>o2sAk0ai7X9</v>
+        <v>oB4qA3ZKs89</v>
       </c>
       <c r="B55" s="5" t="str">
-        <v>[CONFIG] COVAX - Stock on hand - Vaccine1 doses</v>
+        <v>[CONFIG] COVAX - Target people given 1st dose</v>
       </c>
       <c r="C55" s="5" t="str">
-        <v>Stock on hand - Vaccine1 doses</v>
+        <v>Target people given 1st dose</v>
       </c>
       <c r="D55" s="5" t="str">
-        <v>CVX_STOCK_ON_HAND_VACCINE1_DOSES</v>
+        <v>CVX_PEOPLE_1ST_DOSE</v>
       </c>
       <c r="E55" s="5" t="str">
-        <v xml:space="preserve">Stock on-hand at the center after a physical stock count </v>
+        <v>Target people given 1st dose</v>
       </c>
       <c r="F55" s="5" t="str">
-        <v>Stock on hand - Vaccine1 doses</v>
+        <v>Target people given 1st dose</v>
       </c>
       <c r="G55" s="5" t="str">
         <v>1</v>
@@ -3927,7 +3938,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I55" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J55" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3935,31 +3946,31 @@
     </row>
     <row r="56">
       <c r="A56" s="4" t="str">
-        <v>O9HPe4hooiB</v>
+        <v>OkkYt2JpIZ8</v>
       </c>
       <c r="B56" s="4" t="str">
-        <v>[CONFIG] COVAX - Doses discarded by reasons</v>
+        <v>[CONFIG] COVAX - Vaccine 3 uptake (%)</v>
       </c>
       <c r="C56" s="4" t="str">
-        <v>Doses discarded by reasons</v>
+        <v>Vaccine 3 uptake (%)</v>
       </c>
       <c r="D56" s="4" t="str">
-        <v>CVX_DOSES_DISCARDED_BY_REASONS</v>
+        <v>CVX_VACCINE3_UPTAKE_%</v>
       </c>
       <c r="E56" s="4" t="str">
-        <v>Discarded due to expiry, damage, contamination and etc</v>
+        <v>Proportion of people given doses of vaccine3</v>
       </c>
       <c r="F56" s="4" t="str">
-        <v>Vials discarded by reasons</v>
+        <v>Vaccine3 doses given</v>
       </c>
       <c r="G56" s="4" t="str">
-        <v>1</v>
+        <v>Total doses of all vaccines given</v>
       </c>
       <c r="H56" s="4" t="str">
-        <v>Numerator only (number)</v>
+        <v>Percentage</v>
       </c>
       <c r="I56" s="4" t="str">
-        <v>2021-01-21</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J56" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3967,22 +3978,22 @@
     </row>
     <row r="57">
       <c r="A57" s="5" t="str">
-        <v>oB4qA3ZKs89</v>
+        <v>orUc26gd0BF</v>
       </c>
       <c r="B57" s="5" t="str">
-        <v>[CONFIG] COVAX - Target people given 1st dose</v>
+        <v>[CONFIG] COVAX - Closing balance - Vaccine 1 (vials)</v>
       </c>
       <c r="C57" s="5" t="str">
-        <v>Target people given 1st dose</v>
+        <v>Closing balance - Vaccine 1 (vials)</v>
       </c>
       <c r="D57" s="5" t="str">
-        <v>CVX_PEOPLE_1ST_DOSE</v>
+        <v>CVX_CLOSING_BALANCE_VACCINE1_VIALS</v>
       </c>
       <c r="E57" s="5" t="str">
-        <v>Target people given 1st dose</v>
+        <v>(Opening balance+Received)-(Distributed+Redistributed+Discarded)</v>
       </c>
       <c r="F57" s="5" t="str">
-        <v>Target people given 1st dose</v>
+        <v>(Opening balance+Received)-(Distributed+Redistributed+Discarded)</v>
       </c>
       <c r="G57" s="5" t="str">
         <v>1</v>
@@ -3991,7 +4002,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I57" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J57" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3999,31 +4010,31 @@
     </row>
     <row r="58">
       <c r="A58" s="4" t="str">
-        <v>OkkYt2JpIZ8</v>
+        <v>OxPqWqw6hL6</v>
       </c>
       <c r="B58" s="4" t="str">
-        <v>[CONFIG] COVAX - Vaccine3 uptake (%)</v>
+        <v>[CONFIG] COVAX - Frontline healthcare workers given 1st dose</v>
       </c>
       <c r="C58" s="4" t="str">
-        <v>Vaccine3 uptake (%)</v>
+        <v>Frontline healthcare workers given 1st dose</v>
       </c>
       <c r="D58" s="4" t="str">
-        <v>CVX_VACCINE3_UPTAKE_%</v>
+        <v>CVX_FRONTLINE_HCW_1ST_DOSE</v>
       </c>
       <c r="E58" s="4" t="str">
-        <v>Proportion of people given doses of vaccine3</v>
+        <v>Frontline healthcare workers given 1st dose</v>
       </c>
       <c r="F58" s="4" t="str">
-        <v>Vaccine3 doses given</v>
+        <v>Frontline healthcare workers given 1st dose</v>
       </c>
       <c r="G58" s="4" t="str">
-        <v>Total doses of all vaccines given</v>
+        <v>1</v>
       </c>
       <c r="H58" s="4" t="str">
-        <v>Percentage</v>
+        <v>Numerator only (number)</v>
       </c>
       <c r="I58" s="4" t="str">
-        <v>2021-01-21</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J58" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4031,22 +4042,22 @@
     </row>
     <row r="59">
       <c r="A59" s="5" t="str">
-        <v>orUc26gd0BF</v>
+        <v>pqED8vVfjlf</v>
       </c>
       <c r="B59" s="5" t="str">
-        <v>[CONFIG] COVAX - Closing balance - Vaccine1 vials</v>
+        <v>[CONFIG] COVAX - Essential workers given booster dose</v>
       </c>
       <c r="C59" s="5" t="str">
-        <v>Closing balance vials</v>
+        <v>Essential workers given booster dose</v>
       </c>
       <c r="D59" s="5" t="str">
-        <v>CVX_CLOSING_BALANCE_VACCINE1_VIALS</v>
+        <v>CVX_ESSENTIAL_WORKERS_BOOSTER_DOSE</v>
       </c>
       <c r="E59" s="5" t="str">
-        <v>(Opening balance+Received)-(Distributed+Redistributed+Discarded)</v>
+        <v>Essential workers given booster dose</v>
       </c>
       <c r="F59" s="5" t="str">
-        <v>(Opening balance+Received)-(Distributed+Redistributed+Discarded)</v>
+        <v>Essential workers given booster dose</v>
       </c>
       <c r="G59" s="5" t="str">
         <v>1</v>
@@ -4055,7 +4066,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I59" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J59" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4063,22 +4074,22 @@
     </row>
     <row r="60">
       <c r="A60" s="4" t="str">
-        <v>OxPqWqw6hL6</v>
+        <v>q2NHWRFKJIJ</v>
       </c>
       <c r="B60" s="4" t="str">
-        <v>[CONFIG] COVAX - Frontline healthcare workers given 1st dose</v>
+        <v>[CONFIG] COVAX - Redistributed syringes with needle 1ml</v>
       </c>
       <c r="C60" s="4" t="str">
-        <v>Frontline healthcare workers given 1st dose</v>
+        <v>Redistributed syringes with needle 1ml</v>
       </c>
       <c r="D60" s="4" t="str">
-        <v>CVX_FRONTLINE_HCW_1ST_DOSE</v>
+        <v>CVX_REDISTRIBUTED_SYRINGES_WITH_ NEEDLE_1ML</v>
       </c>
       <c r="E60" s="4" t="str">
-        <v>Frontline healthcare workers given 1st dose</v>
+        <v>Redistributed back into the supply chain and is no longer intended for the at the centre</v>
       </c>
       <c r="F60" s="4" t="str">
-        <v>Frontline healthcare workers given 1st dose</v>
+        <v>Redistributed syringes with needle 1ml</v>
       </c>
       <c r="G60" s="4" t="str">
         <v>1</v>
@@ -4087,7 +4098,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I60" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J60" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4095,22 +4106,22 @@
     </row>
     <row r="61">
       <c r="A61" s="5" t="str">
-        <v>pqED8vVfjlf</v>
+        <v>Q5CvJIeZAeh</v>
       </c>
       <c r="B61" s="5" t="str">
-        <v>[CONFIG] COVAX - Essential workers given last dose</v>
+        <v>[CONFIG] COVAX - Redistributed cold box</v>
       </c>
       <c r="C61" s="5" t="str">
-        <v>Essential workers given last dose</v>
+        <v>Redistributed cold box</v>
       </c>
       <c r="D61" s="5" t="str">
-        <v>CVX_ESSENTIAL_WORKERS_LAST_DOSE</v>
+        <v>CVX_REDISTRIBUTED_COLD_BOXES</v>
       </c>
       <c r="E61" s="5" t="str">
-        <v>Essential workers given last dose</v>
+        <v>Redistributed back into the supply chain and is no longer intended for the at the centre</v>
       </c>
       <c r="F61" s="5" t="str">
-        <v>Essential workers given last dose</v>
+        <v>Redistributed cold boxes</v>
       </c>
       <c r="G61" s="5" t="str">
         <v>1</v>
@@ -4119,7 +4130,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I61" s="5" t="str">
-        <v>2021-01-21</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J61" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4127,22 +4138,22 @@
     </row>
     <row r="62">
       <c r="A62" s="4" t="str">
-        <v>q2NHWRFKJIJ</v>
+        <v>q7a0Mh2fRC1</v>
       </c>
       <c r="B62" s="4" t="str">
-        <v>[CONFIG] COVAX - Redistributed syringes with needle 1ml</v>
+        <v>[CONFIG] COVAX - Target people with existing medical conditions given 1st dose</v>
       </c>
       <c r="C62" s="4" t="str">
-        <v>Redistributed syringes with needle 1ml</v>
+        <v>People with existing conditions given 1st dose</v>
       </c>
       <c r="D62" s="4" t="str">
-        <v>CVX_REDISTRIBUTED_SYRINGES_WITH_ NEEDLE_1ML</v>
+        <v>CVX_PEOPLE_WITH_EXISTING_CONDITIONS_1ST_DOSE</v>
       </c>
       <c r="E62" s="4" t="str">
-        <v>Redistributed back into the supply chain and is no longer intended for the at the centre</v>
+        <v>People with existing medical conditions given 1st dose</v>
       </c>
       <c r="F62" s="4" t="str">
-        <v>Redistributed syringes with needle 1ml</v>
+        <v>Target people with existing medical conditions given 1st dose</v>
       </c>
       <c r="G62" s="4" t="str">
         <v>1</v>
@@ -4151,7 +4162,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I62" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J62" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4159,31 +4170,31 @@
     </row>
     <row r="63">
       <c r="A63" s="5" t="str">
-        <v>Q5CvJIeZAeh</v>
+        <v>QH43B8PD9V5</v>
       </c>
       <c r="B63" s="5" t="str">
-        <v>[CONFIG] COVAX - Redistributed cold boxes</v>
+        <v>[CONFIG] COVAX - Proportion of target essential workers given 1st dose</v>
       </c>
       <c r="C63" s="5" t="str">
-        <v>Redistributed cold boxes</v>
+        <v>Target essential workers who received 1st dose (%)</v>
       </c>
       <c r="D63" s="5" t="str">
-        <v>CVX_REDISTRIBUTED_COLD_BOXES</v>
+        <v>CVX_ESS_WORKERS_GIVEN_1ST_DOSE_%</v>
       </c>
       <c r="E63" s="5" t="str">
-        <v>Redistributed back into the supply chain and is no longer intended for the at the centre</v>
+        <v>Proportion of essential workers given 1st dose</v>
       </c>
       <c r="F63" s="5" t="str">
-        <v>Redistributed cold boxes</v>
+        <v>Target essential workers who received 1st dose</v>
       </c>
       <c r="G63" s="5" t="str">
-        <v>1</v>
+        <v>Target essential workers</v>
       </c>
       <c r="H63" s="5" t="str">
-        <v>Numerator only (number)</v>
+        <v>Percentage</v>
       </c>
       <c r="I63" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J63" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4191,22 +4202,22 @@
     </row>
     <row r="64">
       <c r="A64" s="4" t="str">
-        <v>q7a0Mh2fRC1</v>
+        <v>QkFx0Jr0EST</v>
       </c>
       <c r="B64" s="4" t="str">
-        <v>[CONFIG] COVAX - Target people with existing medical conditions given 1st dose</v>
+        <v>[CONFIG] COVAX - Discarded cold box</v>
       </c>
       <c r="C64" s="4" t="str">
-        <v>People with existing conditions given 1st dose</v>
+        <v>Discarded cold box</v>
       </c>
       <c r="D64" s="4" t="str">
-        <v>CVX_PEOPLE_WITH_EXISTING_CONDITIONS_1ST_DOSE</v>
+        <v>CVX_DISCARDED_COLD_BOXES</v>
       </c>
       <c r="E64" s="4" t="str">
-        <v>People with existing medical conditions given 1st dose</v>
+        <v>Discarded due to expiry, damage, contamination and etc</v>
       </c>
       <c r="F64" s="4" t="str">
-        <v>Target people with existing medical conditions given 1st dose</v>
+        <v>Discarded cold boxes</v>
       </c>
       <c r="G64" s="4" t="str">
         <v>1</v>
@@ -4215,7 +4226,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I64" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J64" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4223,31 +4234,31 @@
     </row>
     <row r="65">
       <c r="A65" s="5" t="str">
-        <v>qgyGe1hrTU8</v>
+        <v>qM3QXxyUS64</v>
       </c>
       <c r="B65" s="5" t="str">
-        <v>[CONFIG] COVAX - Proportion of target people with underlying medical conditions given last dose</v>
+        <v>[CONFIG] COVAX - Redistributed safety box</v>
       </c>
       <c r="C65" s="5" t="str">
-        <v>People with existing cond given last dose (%)</v>
+        <v>Redistributed safety box</v>
       </c>
       <c r="D65" s="5" t="str">
-        <v>CVX_EXISTING_CONDS_GIVEN_LAST_DOSE_%</v>
+        <v>CVX_REDISTRIBUTED_SAFETY_BOXES</v>
       </c>
       <c r="E65" s="5" t="str">
-        <v>Proportion of target people with existing medical conditions given last dose</v>
+        <v>Redistributed back into the supply chain and is no longer intended for the at the centre</v>
       </c>
       <c r="F65" s="5" t="str">
-        <v>Target people with existing conditions given last dose</v>
+        <v>Redistributed safety boxes</v>
       </c>
       <c r="G65" s="5" t="str">
-        <v>Target people with underlying medical conditions</v>
+        <v>1</v>
       </c>
       <c r="H65" s="5" t="str">
-        <v>Percentage</v>
+        <v>Numerator only (number)</v>
       </c>
       <c r="I65" s="5" t="str">
-        <v>2021-01-21</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J65" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4255,31 +4266,31 @@
     </row>
     <row r="66">
       <c r="A66" s="4" t="str">
-        <v>QH43B8PD9V5</v>
+        <v>QZritWA9epc</v>
       </c>
       <c r="B66" s="4" t="str">
-        <v>[CONFIG] COVAX - Proportion of target essential workers given 1st dose</v>
+        <v>[CONFIG] COVAX - Redistributed - Vaccine2 doses</v>
       </c>
       <c r="C66" s="4" t="str">
-        <v>Target essential workers who received 1st dose (%)</v>
+        <v>Redistributed - Vaccine2 doses</v>
       </c>
       <c r="D66" s="4" t="str">
-        <v>CVX_ESS_WORKERS_GIVEN_1ST_DOSE_%</v>
+        <v>CVX_REDISTRIBUTED_VACCINE2_DOSES</v>
       </c>
       <c r="E66" s="4" t="str">
-        <v>Proportion of essential workers given 1st dose</v>
+        <v>Redistributed back into the supply chain and is no longer intended for the at the centre</v>
       </c>
       <c r="F66" s="4" t="str">
-        <v>Target essential workers who received 1st dose</v>
+        <v>Redistributed - Vaccine2 doses</v>
       </c>
       <c r="G66" s="4" t="str">
-        <v>Target essential workers</v>
+        <v>1</v>
       </c>
       <c r="H66" s="4" t="str">
-        <v>Percentage</v>
+        <v>Numerator only (number)</v>
       </c>
       <c r="I66" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J66" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4287,31 +4298,31 @@
     </row>
     <row r="67">
       <c r="A67" s="5" t="str">
-        <v>qjnUyy7KWYf</v>
+        <v>RkC5nQeFp1f</v>
       </c>
       <c r="B67" s="5" t="str">
-        <v>[CONFIG] COVAX - Proportion of target essential workers given last dose</v>
+        <v>[CONFIG] COVAX - Doses per vial - Vaccine 2</v>
       </c>
       <c r="C67" s="5" t="str">
-        <v>Target essential workers given last dose (%)</v>
+        <v>Doses per vial - Vaccine 2</v>
       </c>
       <c r="D67" s="5" t="str">
-        <v>CVX_ESS_WORKERS_GIVEN_LAST_DOSE_%</v>
+        <v>CVX_DOSES_IN_A_VIAL_VACCINE2</v>
       </c>
       <c r="E67" s="5" t="str">
-        <v>Proportion of essential workers given last dose</v>
+        <v>Number of doses in a vial - Vaccine2</v>
       </c>
       <c r="F67" s="5" t="str">
-        <v xml:space="preserve">Target essential workers given last dose </v>
+        <v>Doses in a vial - Vaccine2</v>
       </c>
       <c r="G67" s="5" t="str">
-        <v>Target essential workers</v>
+        <v>1</v>
       </c>
       <c r="H67" s="5" t="str">
-        <v>Percentage</v>
+        <v>Numerator only (number)</v>
       </c>
       <c r="I67" s="5" t="str">
-        <v>2021-01-21</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J67" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4319,31 +4330,31 @@
     </row>
     <row r="68">
       <c r="A68" s="4" t="str">
-        <v>QkFx0Jr0EST</v>
+        <v>rms4sR9JeYV</v>
       </c>
       <c r="B68" s="4" t="str">
-        <v>[CONFIG] COVAX - Discarded cold boxes</v>
+        <v>[CONFIG] COVAX - Proportion of target people with underlying medical conditions given 1st dose</v>
       </c>
       <c r="C68" s="4" t="str">
-        <v>Discarded cold boxes</v>
+        <v>People with existing conditions given 1st dose (%)</v>
       </c>
       <c r="D68" s="4" t="str">
-        <v>CVX_DISCARDED_COLD_BOXES</v>
+        <v>CVX_EXISTING_CONDS_GIVEN_1ST_DOSE_%</v>
       </c>
       <c r="E68" s="4" t="str">
-        <v>Discarded due to expiry, damage, contamination and etc</v>
+        <v>Proportion of target people with existing medical conditions given 1st dose</v>
       </c>
       <c r="F68" s="4" t="str">
-        <v>Discarded cold boxes</v>
+        <v>Target people with existing conditions given 1st dose</v>
       </c>
       <c r="G68" s="4" t="str">
-        <v>1</v>
+        <v>Target people with existing medical conditions</v>
       </c>
       <c r="H68" s="4" t="str">
-        <v>Numerator only (number)</v>
+        <v>Percentage</v>
       </c>
       <c r="I68" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J68" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4351,22 +4362,22 @@
     </row>
     <row r="69">
       <c r="A69" s="5" t="str">
-        <v>qM3QXxyUS64</v>
+        <v>RneeVTogdGr</v>
       </c>
       <c r="B69" s="5" t="str">
-        <v>[CONFIG] COVAX - Redistributed safety boxes</v>
+        <v>[CONFIG] COVAX - Opening balance vaccination cards</v>
       </c>
       <c r="C69" s="5" t="str">
-        <v>Redistributed safety boxes</v>
+        <v>Opening balance vaccination cards</v>
       </c>
       <c r="D69" s="5" t="str">
-        <v>CVX_REDISTRIBUTED_SAFETY_BOXES</v>
+        <v>CVX_OPENING_BALANCE_CARDS</v>
       </c>
       <c r="E69" s="5" t="str">
-        <v>Redistributed back into the supply chain and is no longer intended for the at the centre</v>
+        <v>Opening balance equals the physical stock on hand count' of the previous period</v>
       </c>
       <c r="F69" s="5" t="str">
-        <v>Redistributed safety boxes</v>
+        <v>Opening balance vaccination cards</v>
       </c>
       <c r="G69" s="5" t="str">
         <v>1</v>
@@ -4375,7 +4386,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I69" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J69" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4383,31 +4394,31 @@
     </row>
     <row r="70">
       <c r="A70" s="4" t="str">
-        <v>QZritWA9epc</v>
+        <v>SBiW9NeXZeE</v>
       </c>
       <c r="B70" s="4" t="str">
-        <v>[CONFIG] COVAX - Redistributed - Vaccine2 doses</v>
+        <v>[CONFIG] COVAX - Drop out rates among all people targeted</v>
       </c>
       <c r="C70" s="4" t="str">
-        <v>Redistributed - Vaccine2 doses</v>
+        <v>Drop out rates among all (%)</v>
       </c>
       <c r="D70" s="4" t="str">
-        <v>CVX_REDISTRIBUTED_VACCINE2_DOSES</v>
+        <v>CVX_DROPOUT_RATES_AMONG_ALL%</v>
       </c>
       <c r="E70" s="4" t="str">
-        <v>Redistributed back into the supply chain and is no longer intended for the at the centre</v>
+        <v>(1st dose - 2nd dose)/1st dose</v>
       </c>
       <c r="F70" s="4" t="str">
-        <v>Redistributed - Vaccine2 doses</v>
+        <v>Given 1st dose - Given second dose</v>
       </c>
       <c r="G70" s="4" t="str">
-        <v>1</v>
+        <v>Given 1st dose</v>
       </c>
       <c r="H70" s="4" t="str">
-        <v>Numerator only (number)</v>
+        <v>Percentage</v>
       </c>
       <c r="I70" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J70" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4415,31 +4426,31 @@
     </row>
     <row r="71">
       <c r="A71" s="5" t="str">
-        <v>RkC5nQeFp1f</v>
+        <v>sCEtYxBxsIc</v>
       </c>
       <c r="B71" s="5" t="str">
-        <v>[CONFIG] COVAX - Doses in a vial - Vaccine2</v>
+        <v>[CONFIG] COVAX - Drop out rates among people with underlying medical conditions(%)</v>
       </c>
       <c r="C71" s="5" t="str">
-        <v>Doses in a vial - Vaccine2</v>
+        <v>Drop out rates - people with underlying cond (%)</v>
       </c>
       <c r="D71" s="5" t="str">
-        <v>CVX_DOSES_IN_A_VIAL_VACCINE2</v>
+        <v>CVX_DROPOUT_RATES_AMONG_UNDERLYING_CONDs_%</v>
       </c>
       <c r="E71" s="5" t="str">
-        <v>Number of doses in a vial - Vaccine2</v>
+        <v>(1st dose - 2nd dose)/1st dose</v>
       </c>
       <c r="F71" s="5" t="str">
-        <v>Doses in a vial - Vaccine2</v>
+        <v>Given 1st dose - Given second dose</v>
       </c>
       <c r="G71" s="5" t="str">
-        <v>1</v>
+        <v>Given 1st dose</v>
       </c>
       <c r="H71" s="5" t="str">
-        <v>Numerator only (number)</v>
+        <v>Percentage</v>
       </c>
       <c r="I71" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J71" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4447,31 +4458,31 @@
     </row>
     <row r="72">
       <c r="A72" s="4" t="str">
-        <v>rms4sR9JeYV</v>
+        <v>sDWeBvf4rrQ</v>
       </c>
       <c r="B72" s="4" t="str">
-        <v>[CONFIG] COVAX - Proportion of target people with underlying medical conditions given 1st dose</v>
+        <v>[CONFIG] COVAX - Received - Vaccine 1 (doses)</v>
       </c>
       <c r="C72" s="4" t="str">
-        <v>People with existing conditions given 1st dose (%)</v>
+        <v>Received - Vaccine 1 (doses)</v>
       </c>
       <c r="D72" s="4" t="str">
-        <v>CVX_EXISTING_CONDS_GIVEN_1ST_DOSE_%</v>
+        <v>CVX_RECEIVED_VACCINE1_DOSES</v>
       </c>
       <c r="E72" s="4" t="str">
-        <v>Proportion of target people with existing medical conditions given 1st dose</v>
+        <v>Received at the centre</v>
       </c>
       <c r="F72" s="4" t="str">
-        <v>Target people with existing conditions given 1st dose</v>
+        <v>Received - Vaccine1 doses</v>
       </c>
       <c r="G72" s="4" t="str">
-        <v>Target people with existing medical conditions</v>
+        <v>1</v>
       </c>
       <c r="H72" s="4" t="str">
-        <v>Percentage</v>
+        <v>Numerator only (number)</v>
       </c>
       <c r="I72" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J72" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4479,31 +4490,31 @@
     </row>
     <row r="73">
       <c r="A73" s="5" t="str">
-        <v>RneeVTogdGr</v>
+        <v>SvxFYXEwEwh</v>
       </c>
       <c r="B73" s="5" t="str">
-        <v>[CONFIG] COVAX - Opening balance vaccination cards</v>
+        <v>[CONFIG] COVAX - Vaccine stock reporting rates on time</v>
       </c>
       <c r="C73" s="5" t="str">
-        <v>Opening balance vaccination cards</v>
+        <v>Vaccine stock reporting rates on time (%)</v>
       </c>
       <c r="D73" s="5" t="str">
-        <v>CVX_OPENING_BALANCE_CARDS</v>
+        <v>CVX_VAC_STOCK_REPORTING_RATE_ONTIME_%</v>
       </c>
       <c r="E73" s="5" t="str">
-        <v>Opening balance equals the physical stock on hand count' of the previous period</v>
+        <v>Proportion of all vaccination centres that submitted their report on time</v>
       </c>
       <c r="F73" s="5" t="str">
-        <v>Opening balance vaccination cards</v>
+        <v>Actual reports received on time</v>
       </c>
       <c r="G73" s="5" t="str">
-        <v>1</v>
+        <v>Actual reports received</v>
       </c>
       <c r="H73" s="5" t="str">
-        <v>Numerator only (number)</v>
+        <v>Percentage</v>
       </c>
       <c r="I73" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J73" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4511,31 +4522,31 @@
     </row>
     <row r="74">
       <c r="A74" s="4" t="str">
-        <v>SBiW9NeXZeE</v>
+        <v>t4hpTf9Jo4a</v>
       </c>
       <c r="B74" s="4" t="str">
-        <v>[CONFIG] COVAX - Drop out rates among all people targeted</v>
+        <v>[CONFIG] COVAX - Discarded closed vials - Vaccine 3 (doses)</v>
       </c>
       <c r="C74" s="4" t="str">
-        <v>Drop out rates among all (%)</v>
+        <v>Discarded closed vials - Vaccine 3 (doses)</v>
       </c>
       <c r="D74" s="4" t="str">
-        <v>CVX_DROPOUT_RATES_AMONG_ALL%</v>
+        <v>CVX_DISCARDED_VACCINE3_DOSES</v>
       </c>
       <c r="E74" s="4" t="str">
-        <v>(1st dose - last dose)/1st dose</v>
+        <v>Discarded due to expiry, damage, contamination and etc</v>
       </c>
       <c r="F74" s="4" t="str">
-        <v>Given 1st dose - Given last dose</v>
+        <v>Discarded - Vaccine3 doses</v>
       </c>
       <c r="G74" s="4" t="str">
-        <v>Given 1st dose</v>
+        <v>1</v>
       </c>
       <c r="H74" s="4" t="str">
-        <v>Percentage</v>
+        <v>Numerator only (number)</v>
       </c>
       <c r="I74" s="4" t="str">
-        <v>2021-01-21</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J74" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4543,31 +4554,31 @@
     </row>
     <row r="75">
       <c r="A75" s="5" t="str">
-        <v>sCEtYxBxsIc</v>
+        <v>tiFvalDGy3M</v>
       </c>
       <c r="B75" s="5" t="str">
-        <v>[CONFIG] COVAX - Drop out rates among people with underlying medical conditions(%)</v>
+        <v>[CONFIG] COVAX - Redistributed - Vaccine3 doses</v>
       </c>
       <c r="C75" s="5" t="str">
-        <v>Drop out rates - people with underlying cond (%)</v>
+        <v>Redistributed - Vaccine3 doses</v>
       </c>
       <c r="D75" s="5" t="str">
-        <v>CVX_DROPOUT_RATES_AMONG_UNDERLYING_CONDs_%</v>
+        <v>CVX_REDISTRIBUTED_VACCINE3_DOSES</v>
       </c>
       <c r="E75" s="5" t="str">
-        <v>(1st dose - last dose)/1st dose</v>
+        <v>Redistributed back into the supply chain and is no longer intended for the at the centre</v>
       </c>
       <c r="F75" s="5" t="str">
-        <v>Given 1st dose - Given last dose</v>
+        <v>Redistributed - Vaccine3 doses</v>
       </c>
       <c r="G75" s="5" t="str">
-        <v>Given 1st dose</v>
+        <v>1</v>
       </c>
       <c r="H75" s="5" t="str">
-        <v>Percentage</v>
+        <v>Numerator only (number)</v>
       </c>
       <c r="I75" s="5" t="str">
-        <v>2021-01-21</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J75" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4575,22 +4586,22 @@
     </row>
     <row r="76">
       <c r="A76" s="4" t="str">
-        <v>sDWeBvf4rrQ</v>
+        <v>TiylZPMlukw</v>
       </c>
       <c r="B76" s="4" t="str">
-        <v>[CONFIG] COVAX - Received - Vaccine1 doses</v>
+        <v>[CONFIG] COVAX - Received vials</v>
       </c>
       <c r="C76" s="4" t="str">
-        <v>Received - Vaccine1 doses</v>
+        <v>Received vials</v>
       </c>
       <c r="D76" s="4" t="str">
-        <v>CVX_RECEIVED_VACCINE1_DOSES</v>
+        <v>CVX_RECEIVED_VIALS</v>
       </c>
       <c r="E76" s="4" t="str">
         <v>Received at the centre</v>
       </c>
       <c r="F76" s="4" t="str">
-        <v>Received - Vaccine1 doses</v>
+        <v>Received vials</v>
       </c>
       <c r="G76" s="4" t="str">
         <v>1</v>
@@ -4599,7 +4610,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I76" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J76" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4607,31 +4618,31 @@
     </row>
     <row r="77">
       <c r="A77" s="5" t="str">
-        <v>SvxFYXEwEwh</v>
+        <v>TJqiY5fLP8C</v>
       </c>
       <c r="B77" s="5" t="str">
-        <v>[CONFIG] COVAX - Vaccine stock reporting rates on time</v>
+        <v>[CONFIG] COVAX - Target population</v>
       </c>
       <c r="C77" s="5" t="str">
-        <v>Vaccine stock reporting rates on time (%)</v>
+        <v>Target population</v>
       </c>
       <c r="D77" s="5" t="str">
-        <v>CVX_VAC_STOCK_REPORTING_RATE_ONTIME_%</v>
+        <v>CVX_TARGET_POPULATION</v>
       </c>
       <c r="E77" s="5" t="str">
-        <v>Proportion of all vaccination centres that submitted their report on time</v>
+        <v>Target population</v>
       </c>
       <c r="F77" s="5" t="str">
-        <v>Actual reports received on time</v>
+        <v>Target population</v>
       </c>
       <c r="G77" s="5" t="str">
-        <v>Actual reports received</v>
+        <v>1</v>
       </c>
       <c r="H77" s="5" t="str">
-        <v>Percentage</v>
+        <v>Numerator only (number)</v>
       </c>
       <c r="I77" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J77" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4639,31 +4650,31 @@
     </row>
     <row r="78">
       <c r="A78" s="4" t="str">
-        <v>t4hpTf9Jo4a</v>
+        <v>U7Xq3jiK8Fy</v>
       </c>
       <c r="B78" s="4" t="str">
-        <v>[CONFIG] COVAX - Discarded - Vaccine3 doses</v>
+        <v>[CONFIG] COVAX - Proportion of target people given 1st dose</v>
       </c>
       <c r="C78" s="4" t="str">
-        <v>Discarded - Vaccine3 doses</v>
+        <v>Target people given 1st dose (%)</v>
       </c>
       <c r="D78" s="4" t="str">
-        <v>CVX_DISCARDED_VACCINE3_DOSES</v>
+        <v>CVX_PEOPLE_GIVEN_1ST_DOSE_%</v>
       </c>
       <c r="E78" s="4" t="str">
-        <v>Discarded due to expiry, damage, contamination and etc</v>
+        <v>Proportion of target people given 1st dose</v>
       </c>
       <c r="F78" s="4" t="str">
-        <v>Discarded - Vaccine3 doses</v>
+        <v>Target people given 1st dose</v>
       </c>
       <c r="G78" s="4" t="str">
-        <v>1</v>
+        <v>Target population</v>
       </c>
       <c r="H78" s="4" t="str">
-        <v>Numerator only (number)</v>
+        <v>Percentage</v>
       </c>
       <c r="I78" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J78" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4671,22 +4682,22 @@
     </row>
     <row r="79">
       <c r="A79" s="5" t="str">
-        <v>tiFvalDGy3M</v>
+        <v>uhZxrsrhZuy</v>
       </c>
       <c r="B79" s="5" t="str">
-        <v>[CONFIG] COVAX - Redistributed - Vaccine3 doses</v>
+        <v>[CONFIG] COVAX - Closing balance vials</v>
       </c>
       <c r="C79" s="5" t="str">
-        <v>Redistributed - Vaccine3 doses</v>
+        <v>Closing balance vials</v>
       </c>
       <c r="D79" s="5" t="str">
-        <v>CVX_REDISTRIBUTED_VACCINE3_DOSES</v>
+        <v>CVX_CLOSING_BALANCE_VIALS</v>
       </c>
       <c r="E79" s="5" t="str">
-        <v>Redistributed back into the supply chain and is no longer intended for the at the centre</v>
+        <v>(Opening balance+Received)-(Distributed+Redistributed+Discarded)</v>
       </c>
       <c r="F79" s="5" t="str">
-        <v>Redistributed - Vaccine3 doses</v>
+        <v>(Opening balance+Received)-(Distributed+Redistributed+Discarded)</v>
       </c>
       <c r="G79" s="5" t="str">
         <v>1</v>
@@ -4695,7 +4706,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I79" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J79" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4703,22 +4714,22 @@
     </row>
     <row r="80">
       <c r="A80" s="4" t="str">
-        <v>TiylZPMlukw</v>
+        <v>ujhVVQlwTB0</v>
       </c>
       <c r="B80" s="4" t="str">
-        <v>[CONFIG] COVAX - Received vials</v>
+        <v>[CONFIG] COVAX - Opening balance safety box</v>
       </c>
       <c r="C80" s="4" t="str">
-        <v>Received vials</v>
+        <v>Opening balance safety box</v>
       </c>
       <c r="D80" s="4" t="str">
-        <v>CVX_RECEIVED_VIALS</v>
+        <v>CVX_OPENING_BALANCE_SAFETY_BOXES</v>
       </c>
       <c r="E80" s="4" t="str">
-        <v>Received at the centre</v>
+        <v>Opening balance equals the physical 'stock on hand count' of the previous period</v>
       </c>
       <c r="F80" s="4" t="str">
-        <v>Received vials</v>
+        <v>Opening balance safety box</v>
       </c>
       <c r="G80" s="4" t="str">
         <v>1</v>
@@ -4727,7 +4738,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I80" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J80" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4735,22 +4746,22 @@
     </row>
     <row r="81">
       <c r="A81" s="5" t="str">
-        <v>TJqiY5fLP8C</v>
+        <v>UjzjMQpG41z</v>
       </c>
       <c r="B81" s="5" t="str">
-        <v>[CONFIG] COVAX - Target population</v>
+        <v>[CONFIG] COVAX - Stock at hand cold box</v>
       </c>
       <c r="C81" s="5" t="str">
-        <v>Target population</v>
+        <v>Stock at hand cold box</v>
       </c>
       <c r="D81" s="5" t="str">
-        <v>CVX_TARGET_POPULATION</v>
+        <v>CVX_STOCK_AT_HAND_COLD_BOX</v>
       </c>
       <c r="E81" s="5" t="str">
-        <v>Target population</v>
+        <v>Stock on-hand at the center after a physical stock count</v>
       </c>
       <c r="F81" s="5" t="str">
-        <v>Target population</v>
+        <v>Stock on hand cold boxes</v>
       </c>
       <c r="G81" s="5" t="str">
         <v>1</v>
@@ -4759,7 +4770,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I81" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J81" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4767,31 +4778,31 @@
     </row>
     <row r="82">
       <c r="A82" s="4" t="str">
-        <v>u56y5tRtmXY</v>
+        <v>UsMLXbWhhEj</v>
       </c>
       <c r="B82" s="4" t="str">
-        <v>[CONFIG] COVAX - Proportion of target people given last dose</v>
+        <v>[CONFIG] COVAX - Distributed cold box</v>
       </c>
       <c r="C82" s="4" t="str">
-        <v>Target people given last dose (%)</v>
+        <v>Distributed cold box</v>
       </c>
       <c r="D82" s="4" t="str">
-        <v>CVX_PEOPLE_GIVEN_LAST_DOSE_%</v>
+        <v>CVX_DISTRIBUTED_COLD_BOXES</v>
       </c>
       <c r="E82" s="4" t="str">
-        <v>Proportion of target people given last dose</v>
+        <v>Distributed to people receiving the items</v>
       </c>
       <c r="F82" s="4" t="str">
-        <v>Target people given last dose</v>
+        <v>Distributed cold boxes</v>
       </c>
       <c r="G82" s="4" t="str">
-        <v>Target population</v>
+        <v>1</v>
       </c>
       <c r="H82" s="4" t="str">
-        <v>Percentage</v>
+        <v>Numerator only (number)</v>
       </c>
       <c r="I82" s="4" t="str">
-        <v>2021-01-21</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J82" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4799,31 +4810,31 @@
     </row>
     <row r="83">
       <c r="A83" s="5" t="str">
-        <v>U7Xq3jiK8Fy</v>
+        <v>V735nRG647O</v>
       </c>
       <c r="B83" s="5" t="str">
-        <v>[CONFIG] COVAX - Proportion of target people given 1st dose</v>
+        <v>[CONFIG] COVAX - Discarded syringes with needle 1ml</v>
       </c>
       <c r="C83" s="5" t="str">
-        <v>Target people given 1st dose (%)</v>
+        <v>Discarded syringes with needle 1ml</v>
       </c>
       <c r="D83" s="5" t="str">
-        <v>CVX_PEOPLE_GIVEN_1ST_DOSE_%</v>
+        <v>CVX_DISCARDED_SYRINGES_WITH_ NEEDLE_1ML</v>
       </c>
       <c r="E83" s="5" t="str">
-        <v>Proportion of target people given 1st dose</v>
+        <v>Discarded due to expiry, damage, contamination and etc</v>
       </c>
       <c r="F83" s="5" t="str">
-        <v>Target people given 1st dose</v>
+        <v>Discarded syringes with needle 1ml</v>
       </c>
       <c r="G83" s="5" t="str">
-        <v>Target population</v>
+        <v>1</v>
       </c>
       <c r="H83" s="5" t="str">
-        <v>Percentage</v>
+        <v>Numerator only (number)</v>
       </c>
       <c r="I83" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J83" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4831,22 +4842,22 @@
     </row>
     <row r="84">
       <c r="A84" s="4" t="str">
-        <v>uhZxrsrhZuy</v>
+        <v>V8XFjC7JHtx</v>
       </c>
       <c r="B84" s="4" t="str">
-        <v>[CONFIG] COVAX - Closing balance vials</v>
+        <v>[CONFIG] COVAX - Distributed vaccination cards</v>
       </c>
       <c r="C84" s="4" t="str">
-        <v>Closing balance vials</v>
+        <v>Distributed vaccination cards</v>
       </c>
       <c r="D84" s="4" t="str">
-        <v>CVX_CLOSING_BALANCE_VIALS</v>
+        <v>CVX_DISTRIBUTED_CARDS</v>
       </c>
       <c r="E84" s="4" t="str">
-        <v>(Opening balance+Received)-(Distributed+Redistributed+Discarded)</v>
+        <v>Distributed to people receiving the items</v>
       </c>
       <c r="F84" s="4" t="str">
-        <v>(Opening balance+Received)-(Distributed+Redistributed+Discarded)</v>
+        <v>Distributed vaccination cards</v>
       </c>
       <c r="G84" s="4" t="str">
         <v>1</v>
@@ -4855,7 +4866,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I84" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J84" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4863,22 +4874,22 @@
     </row>
     <row r="85">
       <c r="A85" s="5" t="str">
-        <v>ujhVVQlwTB0</v>
+        <v>vBBejr9Qm9y</v>
       </c>
       <c r="B85" s="5" t="str">
-        <v>[CONFIG] COVAX - Opening balance safety boxes</v>
+        <v>[CONFIG] COVAX - Closing balance - Vaccine 3 (vials)</v>
       </c>
       <c r="C85" s="5" t="str">
-        <v>Opening balance safety boxes</v>
+        <v>Closing balance - Vaccine 3 (vials)</v>
       </c>
       <c r="D85" s="5" t="str">
-        <v>CVX_OPENING_BALANCE_SAFETY_BOXES</v>
+        <v>CVX_CLOSING_BALANCE_VACCINE3_VIALS</v>
       </c>
       <c r="E85" s="5" t="str">
-        <v>Opening balance equals the physical 'stock on hand count' of the previous period</v>
+        <v>(Opening balance+Received)-(Distributed+Redistributed+Discarded)</v>
       </c>
       <c r="F85" s="5" t="str">
-        <v>Opening balance safety boxes</v>
+        <v>(Opening balance+Received)-(Distributed+Redistributed+Discarded)</v>
       </c>
       <c r="G85" s="5" t="str">
         <v>1</v>
@@ -4887,7 +4898,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I85" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J85" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4895,22 +4906,22 @@
     </row>
     <row r="86">
       <c r="A86" s="4" t="str">
-        <v>UjzjMQpG41z</v>
+        <v>vBJQTfzca4x</v>
       </c>
       <c r="B86" s="4" t="str">
-        <v>[CONFIG] COVAX - Stock on hand cold boxes</v>
+        <v>[CONFIG] COVAX - Frontline healthcare workers given booster dose</v>
       </c>
       <c r="C86" s="4" t="str">
-        <v>Stock on hand cold boxes</v>
+        <v>Frontline healthcare workers given booster dose</v>
       </c>
       <c r="D86" s="4" t="str">
-        <v>CVX_STOCK_ON_HAND_COLD_BOXES</v>
+        <v>CVX_FRONTLINE_HCW_BOOSTER_DOSE</v>
       </c>
       <c r="E86" s="4" t="str">
-        <v xml:space="preserve">Stock on-hand at the center after a physical stock count </v>
+        <v>Frontline healthcare workers given booster dose</v>
       </c>
       <c r="F86" s="4" t="str">
-        <v>Stock on hand cold boxes</v>
+        <v>Frontline healthcare workers given booster dose</v>
       </c>
       <c r="G86" s="4" t="str">
         <v>1</v>
@@ -4919,7 +4930,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I86" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J86" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4927,22 +4938,22 @@
     </row>
     <row r="87">
       <c r="A87" s="5" t="str">
-        <v>UsMLXbWhhEj</v>
+        <v>VFdnTyYvS5c</v>
       </c>
       <c r="B87" s="5" t="str">
-        <v>[CONFIG] COVAX - Distributed cold boxes</v>
+        <v>[CONFIG] COVAX - Stock at hand vials</v>
       </c>
       <c r="C87" s="5" t="str">
-        <v>Distributed cold boxes</v>
+        <v>Stock at hand vials</v>
       </c>
       <c r="D87" s="5" t="str">
-        <v>CVX_DISTRIBUTED_COLD_BOXES</v>
+        <v>CVX_STOCK_AT_HAND_VIALS</v>
       </c>
       <c r="E87" s="5" t="str">
-        <v>Distributed to people receiving the items</v>
+        <v>Stock on-hand at the center after a physical stock count</v>
       </c>
       <c r="F87" s="5" t="str">
-        <v>Distributed cold boxes</v>
+        <v>Stock on hand vials</v>
       </c>
       <c r="G87" s="5" t="str">
         <v>1</v>
@@ -4951,7 +4962,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I87" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J87" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4959,22 +4970,22 @@
     </row>
     <row r="88">
       <c r="A88" s="4" t="str">
-        <v>V735nRG647O</v>
+        <v>vn6JSZdN0Gq</v>
       </c>
       <c r="B88" s="4" t="str">
-        <v>[CONFIG] COVAX - Discarded syringes with needle 1ml</v>
+        <v>[CONFIG] COVAX - Stockout days cold box</v>
       </c>
       <c r="C88" s="4" t="str">
-        <v>Discarded syringes with needle 1ml</v>
+        <v>Stockout days cold box</v>
       </c>
       <c r="D88" s="4" t="str">
-        <v>CVX_DISCARDED_SYRINGES_WITH_ NEEDLE_1ML</v>
+        <v>CVX_STOCKOUT_DAYS_COLD_BOX</v>
       </c>
       <c r="E88" s="4" t="str">
-        <v>Discarded due to expiry, damage, contamination and etc</v>
+        <v>Days the facility was stocked out of the item</v>
       </c>
       <c r="F88" s="4" t="str">
-        <v>Discarded syringes with needle 1ml</v>
+        <v>Stockout days cold boxes</v>
       </c>
       <c r="G88" s="4" t="str">
         <v>1</v>
@@ -4983,7 +4994,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I88" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J88" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4991,22 +5002,22 @@
     </row>
     <row r="89">
       <c r="A89" s="5" t="str">
-        <v>V8XFjC7JHtx</v>
+        <v>w42k9kZegoW</v>
       </c>
       <c r="B89" s="5" t="str">
-        <v>[CONFIG] COVAX - Distributed vaccination cards</v>
+        <v>[CONFIG] COVAX - Distributed safety box</v>
       </c>
       <c r="C89" s="5" t="str">
-        <v>Distributed vaccination cards</v>
+        <v>Distributed safety box</v>
       </c>
       <c r="D89" s="5" t="str">
-        <v>CVX_DISTRIBUTED_CARDS</v>
+        <v>CVX_DISTRIBUTED_SAFETY_BOXES</v>
       </c>
       <c r="E89" s="5" t="str">
         <v>Distributed to people receiving the items</v>
       </c>
       <c r="F89" s="5" t="str">
-        <v>Distributed vaccination cards</v>
+        <v>Distributed safety boxes</v>
       </c>
       <c r="G89" s="5" t="str">
         <v>1</v>
@@ -5015,7 +5026,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I89" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J89" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5023,22 +5034,22 @@
     </row>
     <row r="90">
       <c r="A90" s="4" t="str">
-        <v>vBBejr9Qm9y</v>
+        <v>wassnxEhpwM</v>
       </c>
       <c r="B90" s="4" t="str">
-        <v>[CONFIG] COVAX - Closing balance - Vaccine3 vials</v>
+        <v>[CONFIG] COVAX - Target essential workers</v>
       </c>
       <c r="C90" s="4" t="str">
-        <v>Closing balance - Vaccine3 vials</v>
+        <v>Target essential workers</v>
       </c>
       <c r="D90" s="4" t="str">
-        <v>CVX_CLOSING_BALANCE_VACCINE3_VIALS</v>
+        <v>CVX_TARGET_ESSENTIAL_WORKERS</v>
       </c>
       <c r="E90" s="4" t="str">
-        <v>(Opening balance+Received)-(Distributed+Redistributed+Discarded)</v>
+        <v>Target essential workers</v>
       </c>
       <c r="F90" s="4" t="str">
-        <v>(Opening balance+Received)-(Distributed+Redistributed+Discarded)</v>
+        <v>Target essential workers</v>
       </c>
       <c r="G90" s="4" t="str">
         <v>1</v>
@@ -5047,7 +5058,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I90" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J90" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5055,22 +5066,22 @@
     </row>
     <row r="91">
       <c r="A91" s="5" t="str">
-        <v>vBJQTfzca4x</v>
+        <v>wcMsZNh0GO0</v>
       </c>
       <c r="B91" s="5" t="str">
-        <v>[CONFIG] COVAX - Frontline healthcare workers given last dose</v>
+        <v>[CONFIG] COVAX - Received safety box</v>
       </c>
       <c r="C91" s="5" t="str">
-        <v>Frontline healthcare workers given last dose</v>
+        <v>Received safety box</v>
       </c>
       <c r="D91" s="5" t="str">
-        <v>CVX_FRONTLINE_HCW_LAST_DOSE</v>
+        <v>CVX_RECEIVED_SAFETY_BOX</v>
       </c>
       <c r="E91" s="5" t="str">
-        <v>Frontline healthcare workers given last dose</v>
+        <v>Received at the centre</v>
       </c>
       <c r="F91" s="5" t="str">
-        <v>Frontline healthcare workers given last dose</v>
+        <v>Received safety boxes</v>
       </c>
       <c r="G91" s="5" t="str">
         <v>1</v>
@@ -5079,7 +5090,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I91" s="5" t="str">
-        <v>2021-01-21</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J91" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5087,22 +5098,22 @@
     </row>
     <row r="92">
       <c r="A92" s="4" t="str">
-        <v>VFdnTyYvS5c</v>
+        <v>WMjFkieChKj</v>
       </c>
       <c r="B92" s="4" t="str">
-        <v>[CONFIG] COVAX - Stock on hand vials</v>
+        <v>[CONFIG] COVAX - Stockout days - Vaccine 2 (vials)</v>
       </c>
       <c r="C92" s="4" t="str">
-        <v>Stock on hand vials</v>
+        <v>Stockout days - Vaccine 2 (vials)</v>
       </c>
       <c r="D92" s="4" t="str">
-        <v>CVX_STOCK_ON_HAND_VIALS</v>
+        <v>CVX_STOCKOUT_DAYS_VACCINE2_VIALS</v>
       </c>
       <c r="E92" s="4" t="str">
-        <v xml:space="preserve">Stock on-hand at the center after a physical stock count </v>
+        <v>Days the centre was stocked out of the item</v>
       </c>
       <c r="F92" s="4" t="str">
-        <v>Stock on hand vials</v>
+        <v>Stockout days - Vaccine2</v>
       </c>
       <c r="G92" s="4" t="str">
         <v>1</v>
@@ -5111,7 +5122,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I92" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J92" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5119,22 +5130,22 @@
     </row>
     <row r="93">
       <c r="A93" s="5" t="str">
-        <v>vn6JSZdN0Gq</v>
+        <v>wpfKN5vD3QG</v>
       </c>
       <c r="B93" s="5" t="str">
-        <v>[CONFIG] COVAX - Stockout days cold boxes</v>
+        <v>[CONFIG] COVAX - Used vials</v>
       </c>
       <c r="C93" s="5" t="str">
-        <v>Stockout days cold boxes</v>
+        <v>Used vials</v>
       </c>
       <c r="D93" s="5" t="str">
-        <v>CVX_STOCKOUT_DAYS_COLD_BOXES</v>
+        <v>CVX_USED_VIALS</v>
       </c>
       <c r="E93" s="5" t="str">
-        <v>Days the facility was stocked out of the item</v>
+        <v>(Opening balance+Received)-(Redistributed+Stock on hand)</v>
       </c>
       <c r="F93" s="5" t="str">
-        <v>Stockout days cold boxes</v>
+        <v>(Opening balance+Received)-(Redistributed+Stock on hand)</v>
       </c>
       <c r="G93" s="5" t="str">
         <v>1</v>
@@ -5143,7 +5154,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I93" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J93" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5151,22 +5162,22 @@
     </row>
     <row r="94">
       <c r="A94" s="4" t="str">
-        <v>w42k9kZegoW</v>
+        <v>X2XYc8WNUY3</v>
       </c>
       <c r="B94" s="4" t="str">
-        <v>[CONFIG] COVAX - Distributed safety boxes</v>
+        <v>[CONFIG] COVAX - Distributed - Vaccine 1 (doses)</v>
       </c>
       <c r="C94" s="4" t="str">
-        <v>Distributed safety boxes</v>
+        <v>Distributed - Vaccine 1 (doses)</v>
       </c>
       <c r="D94" s="4" t="str">
-        <v>CVX_DISTRIBUTED_SAFETY_BOXES</v>
+        <v>CVX_DISTRIBUTED_VACCINE1_DOSES</v>
       </c>
       <c r="E94" s="4" t="str">
-        <v>Distributed to people receiving the items</v>
+        <v>Distributed to people receiving the vaccines</v>
       </c>
       <c r="F94" s="4" t="str">
-        <v>Distributed safety boxes</v>
+        <v>Distributed - Vaccine1 doses</v>
       </c>
       <c r="G94" s="4" t="str">
         <v>1</v>
@@ -5175,7 +5186,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I94" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J94" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5183,22 +5194,22 @@
     </row>
     <row r="95">
       <c r="A95" s="5" t="str">
-        <v>wassnxEhpwM</v>
+        <v>XxmA3VOxZdM</v>
       </c>
       <c r="B95" s="5" t="str">
-        <v>[CONFIG] COVAX - Target essential workers</v>
+        <v>[CONFIG] COVAX - Distributed - Vaccine 3 (doses)</v>
       </c>
       <c r="C95" s="5" t="str">
-        <v>Target essential workers</v>
+        <v>Distributed - Vaccine 3 (doses)</v>
       </c>
       <c r="D95" s="5" t="str">
-        <v>CVX_TARGET_ESSENTIAL_WORKERS</v>
+        <v>CVX_DISTRIBUTED_VACCINE3_DOSES</v>
       </c>
       <c r="E95" s="5" t="str">
-        <v>Target essential workers</v>
+        <v>Distributed to people receiving the vaccines</v>
       </c>
       <c r="F95" s="5" t="str">
-        <v>Target essential workers</v>
+        <v>Distributed - Vaccine3 doses</v>
       </c>
       <c r="G95" s="5" t="str">
         <v>1</v>
@@ -5207,7 +5218,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I95" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J95" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5215,31 +5226,31 @@
     </row>
     <row r="96">
       <c r="A96" s="4" t="str">
-        <v>wcMsZNh0GO0</v>
+        <v>y7uIwU6x8VS</v>
       </c>
       <c r="B96" s="4" t="str">
-        <v>[CONFIG] COVAX - Received safety boxes</v>
+        <v>[CONFIG] COVAX - Vaccine 1 uptake (%)</v>
       </c>
       <c r="C96" s="4" t="str">
-        <v>Received safety boxes</v>
+        <v>Vaccine 1 uptake (%)</v>
       </c>
       <c r="D96" s="4" t="str">
-        <v>CVX_RECEIVED_SAFETY_BOXES</v>
+        <v>CVX_VACCINE1_UPTAKE_%</v>
       </c>
       <c r="E96" s="4" t="str">
-        <v>Received at the centre</v>
+        <v>Proportion of people given doses of vaccine1</v>
       </c>
       <c r="F96" s="4" t="str">
-        <v>Received safety boxes</v>
+        <v>Vaccine1 doses given</v>
       </c>
       <c r="G96" s="4" t="str">
-        <v>1</v>
+        <v>Total doses of all vaccines given</v>
       </c>
       <c r="H96" s="4" t="str">
-        <v>Numerator only (number)</v>
+        <v>Percentage</v>
       </c>
       <c r="I96" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J96" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5247,22 +5258,22 @@
     </row>
     <row r="97">
       <c r="A97" s="5" t="str">
-        <v>WMjFkieChKj</v>
+        <v>yB3Vf9Quskj</v>
       </c>
       <c r="B97" s="5" t="str">
-        <v>[CONFIG] COVAX - Stockout days - Vaccine2 vials</v>
+        <v>[CONFIG] COVAX - Discarded vaccination cards</v>
       </c>
       <c r="C97" s="5" t="str">
-        <v>Stockout days - Vaccine2 vials</v>
+        <v>Discarded vaccination cards</v>
       </c>
       <c r="D97" s="5" t="str">
-        <v>CVX_STOCKOUT_DAYS_VACCINE2_VIALS</v>
+        <v>CVX_DISCARDED_CARDS</v>
       </c>
       <c r="E97" s="5" t="str">
-        <v xml:space="preserve"> Days the centre was stocked out of the item</v>
+        <v>Discarded due to expiry, damage, contamination and etc</v>
       </c>
       <c r="F97" s="5" t="str">
-        <v>Stockout days - Vaccine2</v>
+        <v>Discarded vaccination cards</v>
       </c>
       <c r="G97" s="5" t="str">
         <v>1</v>
@@ -5271,7 +5282,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I97" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J97" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5279,31 +5290,31 @@
     </row>
     <row r="98">
       <c r="A98" s="4" t="str">
-        <v>wpfKN5vD3QG</v>
+        <v>Yb759ffWrrD</v>
       </c>
       <c r="B98" s="4" t="str">
-        <v>[CONFIG] COVAX - Used vials</v>
+        <v>[CONFIG] COVAX - Vaccine usage rate (%)</v>
       </c>
       <c r="C98" s="4" t="str">
+        <v>Vaccine usage rate (%)</v>
+      </c>
+      <c r="D98" s="4" t="str">
+        <v>CVX_ VACCINE_USAGE_RATE_%</v>
+      </c>
+      <c r="E98" s="4" t="str">
+        <v>(Distributed/Used)*100</v>
+      </c>
+      <c r="F98" s="4" t="str">
+        <v>Distributed vials</v>
+      </c>
+      <c r="G98" s="4" t="str">
         <v>Used vials</v>
       </c>
-      <c r="D98" s="4" t="str">
-        <v>CVX_USED_VIALS</v>
-      </c>
-      <c r="E98" s="4" t="str">
-        <v>(Opening balance+Received)-(Redistributed+Stock on hand)</v>
-      </c>
-      <c r="F98" s="4" t="str">
-        <v>(Opening balance+Received)-(Redistributed+Stock on hand)</v>
-      </c>
-      <c r="G98" s="4" t="str">
-        <v>1</v>
-      </c>
       <c r="H98" s="4" t="str">
-        <v>Numerator only (number)</v>
+        <v>Percentage</v>
       </c>
       <c r="I98" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J98" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5311,22 +5322,22 @@
     </row>
     <row r="99">
       <c r="A99" s="5" t="str">
-        <v>X2XYc8WNUY3</v>
+        <v>YBLUIQSCFPJ</v>
       </c>
       <c r="B99" s="5" t="str">
-        <v>[CONFIG] COVAX - Distributed - Vaccine1 doses</v>
+        <v>[CONFIG] COVAX - Closing balance - Vaccine 3 (doses)</v>
       </c>
       <c r="C99" s="5" t="str">
-        <v>Distributed - Vaccine1 doses</v>
+        <v>Closing balance - Vaccine 3 (doses)</v>
       </c>
       <c r="D99" s="5" t="str">
-        <v>CVX_DISTRIBUTED_VACCINE1_DOSES</v>
+        <v>CVX_CLOSING_BALANCE_VACCINE3_DOSES</v>
       </c>
       <c r="E99" s="5" t="str">
-        <v>Distributed to people receiving the vaccines</v>
+        <v>(Opening balance+Received)-(Distributed+Redistributed+Discarded)</v>
       </c>
       <c r="F99" s="5" t="str">
-        <v>Distributed - Vaccine1 doses</v>
+        <v>(Opening balance+Received)-(Distributed+Redistributed+Discarded)</v>
       </c>
       <c r="G99" s="5" t="str">
         <v>1</v>
@@ -5335,7 +5346,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I99" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J99" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5343,22 +5354,22 @@
     </row>
     <row r="100">
       <c r="A100" s="4" t="str">
-        <v>XxmA3VOxZdM</v>
+        <v>yJ9izFBk1bB</v>
       </c>
       <c r="B100" s="4" t="str">
-        <v>[CONFIG] COVAX - Distributed - Vaccine3 doses</v>
+        <v>[CONFIG] COVAX - Closing balance safety boxes</v>
       </c>
       <c r="C100" s="4" t="str">
-        <v>Distributed - Vaccine3 doses</v>
+        <v>Closing balance safety boxes</v>
       </c>
       <c r="D100" s="4" t="str">
-        <v>CVX_DISTRIBUTED_VACCINE3_DOSES</v>
+        <v>CVX_CLOSING_BALANCE_SAFETY_BOXES</v>
       </c>
       <c r="E100" s="4" t="str">
-        <v>Distributed to people receiving the vaccines</v>
+        <v>(Opening balance+Received)-(Distributed+Redistributed+Discarded)</v>
       </c>
       <c r="F100" s="4" t="str">
-        <v>Distributed - Vaccine3 doses</v>
+        <v>(Opening balance+Received)-(Distributed+Redistributed+Discarded)</v>
       </c>
       <c r="G100" s="4" t="str">
         <v>1</v>
@@ -5367,7 +5378,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I100" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J100" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5375,31 +5386,31 @@
     </row>
     <row r="101">
       <c r="A101" s="5" t="str">
-        <v>y7uIwU6x8VS</v>
+        <v>ymno3YCIqbh</v>
       </c>
       <c r="B101" s="5" t="str">
-        <v>[CONFIG] COVAX - Vaccine1 uptake (%)</v>
+        <v>[CONFIG] COVAX - Redistributed vaccination cards</v>
       </c>
       <c r="C101" s="5" t="str">
-        <v>Vaccine 1 uptake (%)</v>
+        <v>Redistributed vaccination cards</v>
       </c>
       <c r="D101" s="5" t="str">
-        <v>CVX_VACCINE1_UPTAKE_%</v>
+        <v>CVX_REDISTRIBUTED_CARDS</v>
       </c>
       <c r="E101" s="5" t="str">
-        <v>Proportion of people given doses of vaccine1</v>
+        <v>Redistributed back into the supply chain and is no longer intended for the at the centre</v>
       </c>
       <c r="F101" s="5" t="str">
-        <v>Vaccine1 doses given</v>
+        <v>Redistributed vaccination cards</v>
       </c>
       <c r="G101" s="5" t="str">
-        <v>Total doses of all vaccines given</v>
+        <v>1</v>
       </c>
       <c r="H101" s="5" t="str">
-        <v>Percentage</v>
+        <v>Numerator only (number)</v>
       </c>
       <c r="I101" s="5" t="str">
-        <v>2021-01-21</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J101" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5407,22 +5418,22 @@
     </row>
     <row r="102">
       <c r="A102" s="4" t="str">
-        <v>yB3Vf9Quskj</v>
+        <v>yuEFomZq3Fh</v>
       </c>
       <c r="B102" s="4" t="str">
-        <v>[CONFIG] COVAX - Discarded vaccination cards</v>
+        <v>[CONFIG] COVAX - Closing balance cold boxes</v>
       </c>
       <c r="C102" s="4" t="str">
-        <v>Discarded vaccination cards</v>
+        <v>Closing balance cold boxes</v>
       </c>
       <c r="D102" s="4" t="str">
-        <v>CVX_DISCARDED_CARDS</v>
+        <v>CVX_CLOSING_BALANCE_COLD_BOXES</v>
       </c>
       <c r="E102" s="4" t="str">
-        <v>Discarded due to expiry, damage, contamination and etc</v>
+        <v>(Opening balance+Received)-(Distributed+Redistributed+Discarded)</v>
       </c>
       <c r="F102" s="4" t="str">
-        <v>Discarded vaccination cards</v>
+        <v>(Opening balance+Received)-(Distributed+Redistributed+Discarded)</v>
       </c>
       <c r="G102" s="4" t="str">
         <v>1</v>
@@ -5431,7 +5442,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I102" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J102" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5439,31 +5450,31 @@
     </row>
     <row r="103">
       <c r="A103" s="5" t="str">
-        <v>Yb759ffWrrD</v>
+        <v>z0zjaGkserE</v>
       </c>
       <c r="B103" s="5" t="str">
-        <v>[CONFIG] COVAX - Vaccine usage rate (%)</v>
+        <v>[CONFIG] COVAX - Discarded safety box</v>
       </c>
       <c r="C103" s="5" t="str">
-        <v>Vaccine usage rate (%)</v>
+        <v>Discarded safety box</v>
       </c>
       <c r="D103" s="5" t="str">
-        <v>CVX_ VACCINE_USAGE_RATE_%</v>
+        <v>CVX_DISCARDED_SAFETY_BOXES</v>
       </c>
       <c r="E103" s="5" t="str">
-        <v>(Distributed/Used)*100</v>
+        <v>Discarded due to expiry, damage, contamination and etc</v>
       </c>
       <c r="F103" s="5" t="str">
-        <v>Distributed vials</v>
+        <v>Discarded safety boxes</v>
       </c>
       <c r="G103" s="5" t="str">
-        <v>Used vials</v>
+        <v>1</v>
       </c>
       <c r="H103" s="5" t="str">
-        <v>Percentage</v>
+        <v>Numerator only (number)</v>
       </c>
       <c r="I103" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J103" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5471,22 +5482,22 @@
     </row>
     <row r="104">
       <c r="A104" s="4" t="str">
-        <v>YBLUIQSCFPJ</v>
+        <v>zcN15JQUWc7</v>
       </c>
       <c r="B104" s="4" t="str">
-        <v>[CONFIG] COVAX - Closing balance - Vaccine3 doses</v>
+        <v>[CONFIG] COVAX - Stock at hand - Vaccine 2 (doses)</v>
       </c>
       <c r="C104" s="4" t="str">
-        <v>Closing balance - Vaccine3 doses</v>
+        <v>Stock at hand - Vaccine 2 (doses)</v>
       </c>
       <c r="D104" s="4" t="str">
-        <v>CVX_CLOSING_BALANCE_VACCINE3_DOSES</v>
+        <v>CVX_STOCK_AT_HAND_VACCINE2_DOSES</v>
       </c>
       <c r="E104" s="4" t="str">
-        <v>(Opening balance+Received)-(Distributed+Redistributed+Discarded)</v>
+        <v>Stock on-hand at the center after a physical stock count</v>
       </c>
       <c r="F104" s="4" t="str">
-        <v>(Opening balance+Received)-(Distributed+Redistributed+Discarded)</v>
+        <v>Stock on hand - Vaccine2 doses</v>
       </c>
       <c r="G104" s="4" t="str">
         <v>1</v>
@@ -5495,7 +5506,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I104" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J104" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5503,31 +5514,31 @@
     </row>
     <row r="105">
       <c r="A105" s="5" t="str">
-        <v>YClBh4hwpk7</v>
+        <v>zdTKcWr73Sk</v>
       </c>
       <c r="B105" s="5" t="str">
-        <v>[CONFIG] COVAX - Proportion of target frontline healthcare workers given last dose</v>
+        <v>[CONFIG] COVAX - Stock at hand syringes with needle 1ml</v>
       </c>
       <c r="C105" s="5" t="str">
-        <v>Frontline healthcare workers given last dose (%)</v>
+        <v>Stock at hand syringes with needle 1ml</v>
       </c>
       <c r="D105" s="5" t="str">
-        <v>CVX_FRONTLINE_HCW_GIVEN_LAST_DOSE_%</v>
+        <v>CVX_STOCK_AT_HAND_SYRINGES_WITH_ NEEDLE_1ML</v>
       </c>
       <c r="E105" s="5" t="str">
-        <v>Proportion of frontline healthcare workers given last dose</v>
+        <v>Stock on-hand at the center after a physical stock count</v>
       </c>
       <c r="F105" s="5" t="str">
-        <v>Target frontline healthcare workers  given last dose</v>
+        <v>Stock on hand syringes with needle 1ml</v>
       </c>
       <c r="G105" s="5" t="str">
-        <v>Target frontline healthcare workers</v>
+        <v>1</v>
       </c>
       <c r="H105" s="5" t="str">
-        <v>Percentage</v>
+        <v>Numerator only (number)</v>
       </c>
       <c r="I105" s="5" t="str">
-        <v>2021-01-21</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J105" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5535,16 +5546,16 @@
     </row>
     <row r="106">
       <c r="A106" s="4" t="str">
-        <v>yJ9izFBk1bB</v>
+        <v>ZEXvmTSnv8c</v>
       </c>
       <c r="B106" s="4" t="str">
-        <v>[CONFIG] COVAX - Closing balance safety boxes</v>
+        <v>[CONFIG] COVAX - Closing balance - Vaccine 2 (doses)</v>
       </c>
       <c r="C106" s="4" t="str">
-        <v>Closing balance safety boxes</v>
+        <v>Closing balance - Vaccine 2 (doses)</v>
       </c>
       <c r="D106" s="4" t="str">
-        <v>CVX_CLOSING_BALANCE_SAFETY_BOXES</v>
+        <v>CVX_CLOSING_BALANCE_VACCINE2_DOSES</v>
       </c>
       <c r="E106" s="4" t="str">
         <v>(Opening balance+Received)-(Distributed+Redistributed+Discarded)</v>
@@ -5559,7 +5570,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I106" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J106" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5567,22 +5578,22 @@
     </row>
     <row r="107">
       <c r="A107" s="5" t="str">
-        <v>ymno3YCIqbh</v>
+        <v>zqTS3RiSL3o</v>
       </c>
       <c r="B107" s="5" t="str">
-        <v>[CONFIG] COVAX - Redistributed vaccination cards</v>
+        <v>[CONFIG] COVAX - Doses per vial - Vaccine 1</v>
       </c>
       <c r="C107" s="5" t="str">
-        <v>Redistributed vaccination cards</v>
+        <v>Doses per vial - Vaccine 1</v>
       </c>
       <c r="D107" s="5" t="str">
-        <v>CVX_REDISTRIBUTED_CARDS</v>
+        <v>CVX_DOSES_IN_A_VIAL_VACCINE1</v>
       </c>
       <c r="E107" s="5" t="str">
-        <v>Redistributed back into the supply chain and is no longer intended for the at the centre</v>
+        <v>Number of doses in a vial - Vaccine1</v>
       </c>
       <c r="F107" s="5" t="str">
-        <v>Redistributed vaccination cards</v>
+        <v>Doses in a vial - Vaccine1</v>
       </c>
       <c r="G107" s="5" t="str">
         <v>1</v>
@@ -5591,7 +5602,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I107" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J107" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5599,22 +5610,22 @@
     </row>
     <row r="108">
       <c r="A108" s="4" t="str">
-        <v>yuEFomZq3Fh</v>
+        <v>zTMJ8UYjlCU</v>
       </c>
       <c r="B108" s="4" t="str">
-        <v>[CONFIG] COVAX - Closing balance cold boxes</v>
+        <v>[CONFIG] COVAX - Opening balance vials</v>
       </c>
       <c r="C108" s="4" t="str">
-        <v>Closing balance cold boxes</v>
+        <v>Opening balance vials</v>
       </c>
       <c r="D108" s="4" t="str">
-        <v>CVX_CLOSING_BALANCE_COLD_BOXES</v>
+        <v>CVX_OPENING_BALANCE_VIALS</v>
       </c>
       <c r="E108" s="4" t="str">
-        <v>(Opening balance+Received)-(Distributed+Redistributed+Discarded)</v>
+        <v>Opening balance equals the physical 'stock on hand count' of the previous day</v>
       </c>
       <c r="F108" s="4" t="str">
-        <v>(Opening balance+Received)-(Distributed+Redistributed+Discarded)</v>
+        <v>Opening balance vials</v>
       </c>
       <c r="G108" s="4" t="str">
         <v>1</v>
@@ -5623,201 +5634,9 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I108" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-28</v>
       </c>
       <c r="J108" s="4" t="str">
-        <v>SKgp2iI0dJp</v>
-      </c>
-    </row>
-    <row r="109">
-      <c r="A109" s="5" t="str">
-        <v>z0zjaGkserE</v>
-      </c>
-      <c r="B109" s="5" t="str">
-        <v>[CONFIG] COVAX - Discarded safety boxes</v>
-      </c>
-      <c r="C109" s="5" t="str">
-        <v>Discarded safety boxes</v>
-      </c>
-      <c r="D109" s="5" t="str">
-        <v>CVX_DISCARDED_SAFETY_BOXES</v>
-      </c>
-      <c r="E109" s="5" t="str">
-        <v>Discarded due to expiry, damage, contamination and etc</v>
-      </c>
-      <c r="F109" s="5" t="str">
-        <v>Discarded safety boxes</v>
-      </c>
-      <c r="G109" s="5" t="str">
-        <v>1</v>
-      </c>
-      <c r="H109" s="5" t="str">
-        <v>Numerator only (number)</v>
-      </c>
-      <c r="I109" s="5" t="str">
-        <v>2021-01-20</v>
-      </c>
-      <c r="J109" s="5" t="str">
-        <v>SKgp2iI0dJp</v>
-      </c>
-    </row>
-    <row r="110">
-      <c r="A110" s="4" t="str">
-        <v>zcN15JQUWc7</v>
-      </c>
-      <c r="B110" s="4" t="str">
-        <v>[CONFIG] COVAX - Stock on hand - Vaccine2 doses</v>
-      </c>
-      <c r="C110" s="4" t="str">
-        <v>Stock on hand - Vaccine2 doses</v>
-      </c>
-      <c r="D110" s="4" t="str">
-        <v>CVX_STOCK_ON_HAND_VACCINE2_DOSES</v>
-      </c>
-      <c r="E110" s="4" t="str">
-        <v xml:space="preserve">Stock on-hand at the center after a physical stock count </v>
-      </c>
-      <c r="F110" s="4" t="str">
-        <v>Stock on hand - Vaccine2 doses</v>
-      </c>
-      <c r="G110" s="4" t="str">
-        <v>1</v>
-      </c>
-      <c r="H110" s="4" t="str">
-        <v>Numerator only (number)</v>
-      </c>
-      <c r="I110" s="4" t="str">
-        <v>2021-01-20</v>
-      </c>
-      <c r="J110" s="4" t="str">
-        <v>SKgp2iI0dJp</v>
-      </c>
-    </row>
-    <row r="111">
-      <c r="A111" s="5" t="str">
-        <v>zdTKcWr73Sk</v>
-      </c>
-      <c r="B111" s="5" t="str">
-        <v>[CONFIG] COVAX - Stock on hand syringes with needle 1ml</v>
-      </c>
-      <c r="C111" s="5" t="str">
-        <v>Stock on hand syringes with needle 1ml</v>
-      </c>
-      <c r="D111" s="5" t="str">
-        <v>CVX_STOCK_ON_HAND_SYRINGES_WITH_ NEEDLE_1ML</v>
-      </c>
-      <c r="E111" s="5" t="str">
-        <v xml:space="preserve">Stock on-hand at the center after a physical stock count </v>
-      </c>
-      <c r="F111" s="5" t="str">
-        <v>Stock on hand syringes with needle 1ml</v>
-      </c>
-      <c r="G111" s="5" t="str">
-        <v>1</v>
-      </c>
-      <c r="H111" s="5" t="str">
-        <v>Numerator only (number)</v>
-      </c>
-      <c r="I111" s="5" t="str">
-        <v>2021-01-20</v>
-      </c>
-      <c r="J111" s="5" t="str">
-        <v>SKgp2iI0dJp</v>
-      </c>
-    </row>
-    <row r="112">
-      <c r="A112" s="4" t="str">
-        <v>ZEXvmTSnv8c</v>
-      </c>
-      <c r="B112" s="4" t="str">
-        <v>[CONFIG] COVAX - Closing balance - Vaccine2 doses</v>
-      </c>
-      <c r="C112" s="4" t="str">
-        <v>Closing balance - Vaccine2 doses</v>
-      </c>
-      <c r="D112" s="4" t="str">
-        <v>CVX_CLOSING_BALANCE_VACCINE2_DOSES</v>
-      </c>
-      <c r="E112" s="4" t="str">
-        <v>(Opening balance+Received)-(Distributed+Redistributed+Discarded)</v>
-      </c>
-      <c r="F112" s="4" t="str">
-        <v>(Opening balance+Received)-(Distributed+Redistributed+Discarded)</v>
-      </c>
-      <c r="G112" s="4" t="str">
-        <v>1</v>
-      </c>
-      <c r="H112" s="4" t="str">
-        <v>Numerator only (number)</v>
-      </c>
-      <c r="I112" s="4" t="str">
-        <v>2021-01-20</v>
-      </c>
-      <c r="J112" s="4" t="str">
-        <v>SKgp2iI0dJp</v>
-      </c>
-    </row>
-    <row r="113">
-      <c r="A113" s="5" t="str">
-        <v>zqTS3RiSL3o</v>
-      </c>
-      <c r="B113" s="5" t="str">
-        <v>[CONFIG] COVAX - Doses in a vial - Vaccine1</v>
-      </c>
-      <c r="C113" s="5" t="str">
-        <v>Doses in a vial - Vaccine1</v>
-      </c>
-      <c r="D113" s="5" t="str">
-        <v>CVX_DOSES_IN_A_VIAL_VACCINE1</v>
-      </c>
-      <c r="E113" s="5" t="str">
-        <v>Number of doses in a vial - Vaccine1</v>
-      </c>
-      <c r="F113" s="5" t="str">
-        <v>Doses in a vial - Vaccine1</v>
-      </c>
-      <c r="G113" s="5" t="str">
-        <v>1</v>
-      </c>
-      <c r="H113" s="5" t="str">
-        <v>Numerator only (number)</v>
-      </c>
-      <c r="I113" s="5" t="str">
-        <v>2021-01-20</v>
-      </c>
-      <c r="J113" s="5" t="str">
-        <v>SKgp2iI0dJp</v>
-      </c>
-    </row>
-    <row r="114">
-      <c r="A114" s="4" t="str">
-        <v>zTMJ8UYjlCU</v>
-      </c>
-      <c r="B114" s="4" t="str">
-        <v>[CONFIG] COVAX - Opening balance vials</v>
-      </c>
-      <c r="C114" s="4" t="str">
-        <v>Opening balance vials</v>
-      </c>
-      <c r="D114" s="4" t="str">
-        <v>CVX_OPENING_BALANCE_VIALS</v>
-      </c>
-      <c r="E114" s="4" t="str">
-        <v>Opening balance equals the physical 'stock on hand count' of the previous day</v>
-      </c>
-      <c r="F114" s="4" t="str">
-        <v>Opening balance vials</v>
-      </c>
-      <c r="G114" s="4" t="str">
-        <v>1</v>
-      </c>
-      <c r="H114" s="4" t="str">
-        <v>Numerator only (number)</v>
-      </c>
-      <c r="I114" s="4" t="str">
-        <v>2021-01-20</v>
-      </c>
-      <c r="J114" s="4" t="str">
         <v>SKgp2iI0dJp</v>
       </c>
     </row>
@@ -5860,7 +5679,7 @@
         <v>100</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2021-01-18</v>
+        <v>2021-01-28</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>hmSnCXmLYwt</v>
@@ -5874,7 +5693,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>2021-01-18</v>
+        <v>2021-01-28</v>
       </c>
       <c r="D3" s="5" t="str">
         <v>kHy61PbChXr</v>

</xml_diff>

<commit_message>
feat: Update COVAX_AGG packages for DHIS2 v2.30 & v2.33
</commit_message>
<xml_diff>
--- a/metadata/COVAX_AGG/COVAX_AGG_DASHBOARD_V1_DHIS2.30/reference.xlsx
+++ b/metadata/COVAX_AGG/COVAX_AGG_DASHBOARD_V1_DHIS2.30/reference.xlsx
@@ -491,7 +491,7 @@
         <v>Identifier</v>
       </c>
       <c r="B7" s="5" t="str">
-        <v>COVAX_AGG_DASHBOARD_V1.0_DHIS2.30_2021-01-29T11:09</v>
+        <v>COVAX_AGG_DASHBOARD_V1.0_DHIS2.30_2021-02-02T12:36</v>
       </c>
     </row>
   </sheetData>
@@ -932,7 +932,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2021-01-19</v>
+        <v>2021-01-29</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>CwgW21jWHz1</v>
@@ -946,7 +946,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>2021-01-19</v>
+        <v>2021-01-29</v>
       </c>
       <c r="D3" s="5" t="str">
         <v>iBwXpDzZJ4M</v>
@@ -960,7 +960,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>2021-01-19</v>
+        <v>2021-01-29</v>
       </c>
       <c r="D4" s="4" t="str">
         <v>IC3e1YTilA3</v>
@@ -974,7 +974,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>2021-01-19</v>
+        <v>2021-01-29</v>
       </c>
       <c r="D5" s="5" t="str">
         <v>L2geQCvt3m9</v>
@@ -988,7 +988,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>2021-01-19</v>
+        <v>2021-01-29</v>
       </c>
       <c r="D6" s="4" t="str">
         <v>laDW4fMp78v</v>
@@ -1002,7 +1002,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>2021-01-19</v>
+        <v>2021-01-29</v>
       </c>
       <c r="D7" s="5" t="str">
         <v>MeqsIPI7jsf</v>
@@ -1016,7 +1016,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-02-01</v>
       </c>
       <c r="D8" s="4" t="str">
         <v>NBIo8UnkJsU</v>
@@ -1030,7 +1030,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>2021-01-19</v>
+        <v>2021-01-29</v>
       </c>
       <c r="D9" s="5" t="str">
         <v>oP1h3CJEzP2</v>
@@ -1044,7 +1044,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>2021-01-19</v>
+        <v>2021-01-29</v>
       </c>
       <c r="D10" s="4" t="str">
         <v>sGJvgqCpGHn</v>
@@ -1058,7 +1058,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C11" s="5" t="str">
-        <v>2021-01-22</v>
+        <v>2021-01-29</v>
       </c>
       <c r="D11" s="5" t="str">
         <v>T60YVx3ISwD</v>
@@ -1072,7 +1072,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C12" s="4" t="str">
-        <v>2021-01-21</v>
+        <v>2021-01-29</v>
       </c>
       <c r="D12" s="4" t="str">
         <v>UEnas3PpETN</v>
@@ -1086,7 +1086,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C13" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-29</v>
       </c>
       <c r="D13" s="5" t="str">
         <v>vKavKhPWSRc</v>
@@ -1131,7 +1131,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2021-01-27</v>
+        <v>2021-02-01</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>q24wzRQtygl</v>
@@ -1145,7 +1145,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-31</v>
       </c>
       <c r="D3" s="5" t="str">
         <v>UAxSsG1vtda</v>
@@ -1190,7 +1190,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2021-01-21</v>
+        <v>2021-01-31</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>IAmP71D6zQV</v>
@@ -1204,7 +1204,7 @@
         <v xml:space="preserve"> </v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>2021-01-21</v>
+        <v>2021-01-31</v>
       </c>
       <c r="D3" s="5" t="str">
         <v>Sg5FrsMduxN</v>
@@ -1533,7 +1533,7 @@
         <v>COVAX admin</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-31</v>
       </c>
       <c r="C2" s="4" t="str">
         <v>e2QMDWpq88P</v>
@@ -1544,7 +1544,7 @@
         <v>COVAX capture</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>2021-01-20</v>
+        <v>2021-01-31</v>
       </c>
       <c r="C3" s="5" t="str">
         <v>I9x6Bd4MwXc</v>
@@ -1555,7 +1555,7 @@
         <v>COVAX access</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>2021-01-21</v>
+        <v>2021-01-31</v>
       </c>
       <c r="C4" s="4" t="str">
         <v>OeiDCnG3Pv2</v>
@@ -1638,7 +1638,7 @@
         <v>Doses in a vial - Vaccine1</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2021-01-18</v>
+        <v>2021-01-29</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>fyC1NhjpBH5</v>
@@ -1652,7 +1652,7 @@
         <v>Doses in a vial - Vaccine2</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>2021-01-18</v>
+        <v>2021-01-29</v>
       </c>
       <c r="D3" s="5" t="str">
         <v>GhXdnHkmph9</v>
@@ -1666,7 +1666,7 @@
         <v>Doses in a vial - Vaccine3</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>2021-01-18</v>
+        <v>2021-01-29</v>
       </c>
       <c r="D4" s="4" t="str">
         <v>zp3l4iQWPLh</v>
@@ -1704,7 +1704,7 @@
         <v>COVID19 Vaccines</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2021-01-18</v>
+        <v>2021-01-29</v>
       </c>
       <c r="C2" s="4" t="str">
         <v>dX05HKf9jgk</v>
@@ -1715,7 +1715,7 @@
         <v>Vial condition</v>
       </c>
       <c r="B3" s="5" t="str">
-        <v>2021-01-18</v>
+        <v>2021-01-29</v>
       </c>
       <c r="C3" s="5" t="str">
         <v>flirf9mAeha</v>
@@ -1726,7 +1726,7 @@
         <v>Age(&lt;60-60+years)</v>
       </c>
       <c r="B4" s="4" t="str">
-        <v>2021-01-18</v>
+        <v>2021-01-29</v>
       </c>
       <c r="C4" s="4" t="str">
         <v>hEcLht1oMFl</v>
@@ -1737,7 +1737,7 @@
         <v>AEFI Severity</v>
       </c>
       <c r="B5" s="5" t="str">
-        <v>2021-01-18</v>
+        <v>2021-01-29</v>
       </c>
       <c r="C5" s="5" t="str">
         <v>lKWQD9CDlOA</v>
@@ -1748,7 +1748,7 @@
         <v>Wastage reasons</v>
       </c>
       <c r="B6" s="4" t="str">
-        <v>2021-01-19</v>
+        <v>2021-01-29</v>
       </c>
       <c r="C6" s="4" t="str">
         <v>mytJKrvlNuF</v>
@@ -1793,7 +1793,7 @@
         <v>Partial use</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2021-01-18</v>
+        <v>2021-01-29</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>A3jbi9q2pvX</v>
@@ -1807,7 +1807,7 @@
         <v>Serious AEFI</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>2021-01-18</v>
+        <v>2021-01-29</v>
       </c>
       <c r="D3" s="5" t="str">
         <v>aHtHUdheUX7</v>
@@ -1821,7 +1821,7 @@
         <v>Open vial</v>
       </c>
       <c r="C4" s="4" t="str">
-        <v>2021-01-18</v>
+        <v>2021-01-29</v>
       </c>
       <c r="D4" s="4" t="str">
         <v>B1GRrudW4kx</v>
@@ -1835,7 +1835,7 @@
         <v>Other reason</v>
       </c>
       <c r="C5" s="5" t="str">
-        <v>2021-01-18</v>
+        <v>2021-01-29</v>
       </c>
       <c r="D5" s="5" t="str">
         <v>CcM1wEkrHwA</v>
@@ -1849,7 +1849,7 @@
         <v>Color change (VVM)</v>
       </c>
       <c r="C6" s="4" t="str">
-        <v>2021-01-18</v>
+        <v>2021-01-29</v>
       </c>
       <c r="D6" s="4" t="str">
         <v>diTeRoy0yzo</v>
@@ -1863,7 +1863,7 @@
         <v>Vaccine2</v>
       </c>
       <c r="C7" s="5" t="str">
-        <v>2021-01-18</v>
+        <v>2021-01-29</v>
       </c>
       <c r="D7" s="5" t="str">
         <v>FNFBfAafW1b</v>
@@ -1877,7 +1877,7 @@
         <v>0-59 y</v>
       </c>
       <c r="C8" s="4" t="str">
-        <v>2021-01-27</v>
+        <v>2021-01-29</v>
       </c>
       <c r="D8" s="4" t="str">
         <v>fqborXHhXZG</v>
@@ -1891,7 +1891,7 @@
         <v>60+ y</v>
       </c>
       <c r="C9" s="5" t="str">
-        <v>2021-01-18</v>
+        <v>2021-01-29</v>
       </c>
       <c r="D9" s="5" t="str">
         <v>hEct0AAbPAw</v>
@@ -1905,7 +1905,7 @@
         <v>Vaccine3</v>
       </c>
       <c r="C10" s="4" t="str">
-        <v>2021-01-18</v>
+        <v>2021-01-29</v>
       </c>
       <c r="D10" s="4" t="str">
         <v>IIUfyc2Pe6x</v>
@@ -1919,7 +1919,7 @@
         <v>Contamination</v>
       </c>
       <c r="C11" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="D11" s="5" t="str">
         <v>KS058ZLL570</v>
@@ -1933,7 +1933,7 @@
         <v>Vaccine1</v>
       </c>
       <c r="C12" s="4" t="str">
-        <v>2021-01-18</v>
+        <v>2021-01-29</v>
       </c>
       <c r="D12" s="4" t="str">
         <v>TJHsOAXOi3f</v>
@@ -1947,7 +1947,7 @@
         <v>Non-Serious AEFI</v>
       </c>
       <c r="C13" s="5" t="str">
-        <v>2021-01-18</v>
+        <v>2021-01-29</v>
       </c>
       <c r="D13" s="5" t="str">
         <v>uOiOUtqUZdY</v>
@@ -1961,7 +1961,7 @@
         <v>Closed vial</v>
       </c>
       <c r="C14" s="4" t="str">
-        <v>2021-01-18</v>
+        <v>2021-01-29</v>
       </c>
       <c r="D14" s="4" t="str">
         <v>uWJm7E7Jtgk</v>
@@ -1975,7 +1975,7 @@
         <v>Expiry</v>
       </c>
       <c r="C15" s="5" t="str">
-        <v>2021-01-18</v>
+        <v>2021-01-29</v>
       </c>
       <c r="D15" s="5" t="str">
         <v>ZyZJL43yTIM</v>
@@ -2155,7 +2155,7 @@
         <v/>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2242,7 +2242,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I2" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J2" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2274,7 +2274,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I3" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J3" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2306,7 +2306,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I4" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J4" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2338,7 +2338,7 @@
         <v>Percentage</v>
       </c>
       <c r="I5" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J5" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2370,7 +2370,7 @@
         <v>Percentage</v>
       </c>
       <c r="I6" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J6" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2390,10 +2390,10 @@
         <v>CVX_STOCK_AT_HAND_SAFETY_BOX</v>
       </c>
       <c r="E7" s="5" t="str">
-        <v>Stock on-hand at the center after a physical stock count</v>
+        <v>Stock at hand at the center after a physical stock count</v>
       </c>
       <c r="F7" s="5" t="str">
-        <v>Stock on hand safety boxes</v>
+        <v>Stock at hand safety boxes</v>
       </c>
       <c r="G7" s="5" t="str">
         <v>1</v>
@@ -2402,7 +2402,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I7" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J7" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2434,7 +2434,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I8" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J8" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2466,7 +2466,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I9" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J9" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2498,7 +2498,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I10" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J10" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2530,7 +2530,7 @@
         <v>Percentage</v>
       </c>
       <c r="I11" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J11" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2562,7 +2562,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I12" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J12" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2594,7 +2594,7 @@
         <v>Percentage</v>
       </c>
       <c r="I13" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J13" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2626,7 +2626,7 @@
         <v>Percentage</v>
       </c>
       <c r="I14" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J14" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2658,7 +2658,7 @@
         <v>Percentage</v>
       </c>
       <c r="I15" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J15" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2690,7 +2690,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I16" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J16" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2710,10 +2710,10 @@
         <v>CVX_STOCK_AT_HAND_VACCINE3_DOSES</v>
       </c>
       <c r="E17" s="5" t="str">
-        <v>Stock on-hand at the center after a physical stock count</v>
+        <v>Stock at hand at the center after a physical stock count</v>
       </c>
       <c r="F17" s="5" t="str">
-        <v>Stock on hand - Vaccine3 doses</v>
+        <v>Stock at hand - Vaccine 3 doses</v>
       </c>
       <c r="G17" s="5" t="str">
         <v>1</v>
@@ -2722,7 +2722,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I17" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J17" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2754,7 +2754,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I18" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J18" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2786,7 +2786,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I19" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J19" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2818,7 +2818,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I20" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J20" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2850,7 +2850,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I21" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J21" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2882,7 +2882,7 @@
         <v>Percentage</v>
       </c>
       <c r="I22" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J22" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2914,7 +2914,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I23" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J23" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2946,7 +2946,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I24" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J24" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2978,7 +2978,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I25" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J25" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -2998,10 +2998,10 @@
         <v>CVX_STOCK_AT_HAND_CARDS</v>
       </c>
       <c r="E26" s="4" t="str">
-        <v>Stock on-hand at the center after a physical stock count</v>
+        <v>Stock at hand at the center after a physical stock count</v>
       </c>
       <c r="F26" s="4" t="str">
-        <v>Stock on hand vaccination cards</v>
+        <v>Stock at hand vaccination cards</v>
       </c>
       <c r="G26" s="4" t="str">
         <v>1</v>
@@ -3010,7 +3010,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I26" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J26" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3042,7 +3042,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I27" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J27" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3074,7 +3074,7 @@
         <v>Percentage</v>
       </c>
       <c r="I28" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J28" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3106,7 +3106,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I29" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J29" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3138,7 +3138,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I30" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J30" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3170,7 +3170,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I31" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J31" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3202,7 +3202,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I32" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J32" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3234,7 +3234,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I33" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J33" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3266,7 +3266,7 @@
         <v>Percentage</v>
       </c>
       <c r="I34" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J34" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3298,7 +3298,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I35" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J35" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3330,7 +3330,7 @@
         <v>Percentage</v>
       </c>
       <c r="I36" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J36" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3362,7 +3362,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I37" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J37" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3394,7 +3394,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I38" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J38" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3426,7 +3426,7 @@
         <v>Percentage</v>
       </c>
       <c r="I39" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J39" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3458,7 +3458,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I40" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J40" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3490,7 +3490,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I41" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J41" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3522,7 +3522,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I42" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J42" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3554,7 +3554,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I43" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J43" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3586,7 +3586,7 @@
         <v>Percentage</v>
       </c>
       <c r="I44" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J44" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3618,7 +3618,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I45" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J45" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3650,7 +3650,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I46" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J46" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3682,7 +3682,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I47" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J47" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3714,7 +3714,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I48" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J48" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3746,7 +3746,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I49" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J49" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3778,7 +3778,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I50" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J50" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3810,7 +3810,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I51" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J51" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3842,7 +3842,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I52" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J52" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3862,10 +3862,10 @@
         <v>CVX_STOCK_AT_HAND_VACCINE1_DOSES</v>
       </c>
       <c r="E53" s="5" t="str">
-        <v>Stock on-hand at the center after a physical stock count</v>
+        <v>Stock at hand at the center after a physical stock count</v>
       </c>
       <c r="F53" s="5" t="str">
-        <v>Stock on hand - Vaccine1 doses</v>
+        <v>Stock at hand - Vaccine 1 doses</v>
       </c>
       <c r="G53" s="5" t="str">
         <v>1</v>
@@ -3874,7 +3874,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I53" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J53" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3906,7 +3906,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I54" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J54" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3938,7 +3938,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I55" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J55" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -3970,7 +3970,7 @@
         <v>Percentage</v>
       </c>
       <c r="I56" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J56" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4002,7 +4002,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I57" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J57" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4034,7 +4034,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I58" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J58" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4066,7 +4066,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I59" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J59" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4098,7 +4098,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I60" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J60" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4130,7 +4130,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I61" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J61" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4162,7 +4162,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I62" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J62" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4194,7 +4194,7 @@
         <v>Percentage</v>
       </c>
       <c r="I63" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J63" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4226,7 +4226,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I64" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J64" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4258,7 +4258,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I65" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J65" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4290,7 +4290,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I66" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J66" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4322,7 +4322,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I67" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J67" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4354,7 +4354,7 @@
         <v>Percentage</v>
       </c>
       <c r="I68" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J68" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4386,7 +4386,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I69" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J69" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4418,7 +4418,7 @@
         <v>Percentage</v>
       </c>
       <c r="I70" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J70" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4450,7 +4450,7 @@
         <v>Percentage</v>
       </c>
       <c r="I71" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J71" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4482,7 +4482,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I72" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J72" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4514,7 +4514,7 @@
         <v>Percentage</v>
       </c>
       <c r="I73" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J73" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4546,7 +4546,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I74" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J74" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4578,7 +4578,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I75" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J75" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4610,7 +4610,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I76" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J76" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4642,7 +4642,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I77" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J77" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4674,7 +4674,7 @@
         <v>Percentage</v>
       </c>
       <c r="I78" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J78" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4706,7 +4706,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I79" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J79" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4738,7 +4738,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I80" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J80" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4758,10 +4758,10 @@
         <v>CVX_STOCK_AT_HAND_COLD_BOX</v>
       </c>
       <c r="E81" s="5" t="str">
-        <v>Stock on-hand at the center after a physical stock count</v>
+        <v>Stock at hand at the center after a physical stock count</v>
       </c>
       <c r="F81" s="5" t="str">
-        <v>Stock on hand cold boxes</v>
+        <v>Stock at hand cold boxes</v>
       </c>
       <c r="G81" s="5" t="str">
         <v>1</v>
@@ -4770,7 +4770,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I81" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J81" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4802,7 +4802,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I82" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J82" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4834,7 +4834,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I83" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J83" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4866,7 +4866,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I84" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J84" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4898,7 +4898,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I85" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J85" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4930,7 +4930,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I86" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J86" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4950,10 +4950,10 @@
         <v>CVX_STOCK_AT_HAND_VIALS</v>
       </c>
       <c r="E87" s="5" t="str">
-        <v>Stock on-hand at the center after a physical stock count</v>
+        <v>Stock at hand at the center after a physical stock count</v>
       </c>
       <c r="F87" s="5" t="str">
-        <v>Stock on hand vials</v>
+        <v>Stock at hand vials</v>
       </c>
       <c r="G87" s="5" t="str">
         <v>1</v>
@@ -4962,7 +4962,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I87" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J87" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -4994,7 +4994,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I88" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J88" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5026,7 +5026,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I89" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J89" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5058,7 +5058,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I90" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J90" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5090,7 +5090,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I91" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J91" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5122,7 +5122,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I92" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J92" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5154,7 +5154,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I93" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J93" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5186,7 +5186,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I94" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J94" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5218,7 +5218,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I95" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J95" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5250,7 +5250,7 @@
         <v>Percentage</v>
       </c>
       <c r="I96" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J96" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5282,7 +5282,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I97" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J97" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5314,7 +5314,7 @@
         <v>Percentage</v>
       </c>
       <c r="I98" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J98" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5346,7 +5346,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I99" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J99" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5378,7 +5378,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I100" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J100" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5410,7 +5410,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I101" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J101" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5442,7 +5442,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I102" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J102" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5474,7 +5474,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I103" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J103" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5494,10 +5494,10 @@
         <v>CVX_STOCK_AT_HAND_VACCINE2_DOSES</v>
       </c>
       <c r="E104" s="4" t="str">
-        <v>Stock on-hand at the center after a physical stock count</v>
+        <v>Stock at hand at the center after a physical stock count</v>
       </c>
       <c r="F104" s="4" t="str">
-        <v>Stock on hand - Vaccine2 doses</v>
+        <v>Stock at hand - Vaccine 2 doses</v>
       </c>
       <c r="G104" s="4" t="str">
         <v>1</v>
@@ -5506,7 +5506,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I104" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J104" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5526,10 +5526,10 @@
         <v>CVX_STOCK_AT_HAND_SYRINGES_WITH_ NEEDLE_1ML</v>
       </c>
       <c r="E105" s="5" t="str">
-        <v>Stock on-hand at the center after a physical stock count</v>
+        <v>Stock at hand at the center after a physical stock count</v>
       </c>
       <c r="F105" s="5" t="str">
-        <v>Stock on hand syringes with needle 1ml</v>
+        <v>Stock at hand syringes with needle 1ml</v>
       </c>
       <c r="G105" s="5" t="str">
         <v>1</v>
@@ -5538,7 +5538,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I105" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J105" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5570,7 +5570,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I106" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J106" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5602,7 +5602,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I107" s="5" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J107" s="5" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5634,7 +5634,7 @@
         <v>Numerator only (number)</v>
       </c>
       <c r="I108" s="4" t="str">
-        <v>2021-01-29</v>
+        <v>2021-02-01</v>
       </c>
       <c r="J108" s="4" t="str">
         <v>SKgp2iI0dJp</v>
@@ -5679,7 +5679,7 @@
         <v>100</v>
       </c>
       <c r="C2" s="4" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="D2" s="4" t="str">
         <v>hmSnCXmLYwt</v>
@@ -5693,7 +5693,7 @@
         <v>1</v>
       </c>
       <c r="C3" s="5" t="str">
-        <v>2021-01-28</v>
+        <v>2021-01-29</v>
       </c>
       <c r="D3" s="5" t="str">
         <v>kHy61PbChXr</v>
@@ -5731,7 +5731,7 @@
         <v>COVAX - Vaccination</v>
       </c>
       <c r="B2" s="4" t="str">
-        <v>2021-01-22</v>
+        <v>2021-01-29</v>
       </c>
       <c r="C2" s="4" t="str">
         <v>fya0FUpbxX9</v>

</xml_diff>